<commit_message>
Clustering sur ACP et finalisation
</commit_message>
<xml_diff>
--- a/DonnéesFinales.xlsx
+++ b/DonnéesFinales.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="351" uniqueCount="187">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="354" uniqueCount="190">
   <si>
     <t>Continent</t>
   </si>
@@ -50,6 +50,15 @@
   </si>
   <si>
     <t>Kmeans</t>
+  </si>
+  <si>
+    <t>F1</t>
+  </si>
+  <si>
+    <t>F2</t>
+  </si>
+  <si>
+    <t>ACP</t>
   </si>
   <si>
     <t>Zone</t>
@@ -932,15 +941,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:M170"/>
+  <dimension ref="A1:P170"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:13">
+    <row r="1" spans="1:16">
       <c r="A1" s="1" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>0</v>
@@ -978,13 +987,22 @@
       <c r="M1" s="1" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="2" spans="1:13">
+      <c r="N1" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="O1" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="P1" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="2" spans="1:16">
       <c r="A2" s="1" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="B2" t="s">
-        <v>182</v>
+        <v>185</v>
       </c>
       <c r="C2">
         <v>3.39</v>
@@ -1019,13 +1037,22 @@
       <c r="M2">
         <v>1</v>
       </c>
-    </row>
-    <row r="3" spans="1:13">
+      <c r="N2">
+        <v>-3.513882045892454</v>
+      </c>
+      <c r="O2">
+        <v>-0.02767140267819108</v>
+      </c>
+      <c r="P2">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="3" spans="1:16">
       <c r="A3" s="1" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="B3" t="s">
-        <v>183</v>
+        <v>186</v>
       </c>
       <c r="C3">
         <v>1.61</v>
@@ -1060,13 +1087,22 @@
       <c r="M3">
         <v>2</v>
       </c>
-    </row>
-    <row r="4" spans="1:13">
+      <c r="N3">
+        <v>-0.2430651747344462</v>
+      </c>
+      <c r="O3">
+        <v>-0.01428616590036348</v>
+      </c>
+      <c r="P3">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="4" spans="1:16">
       <c r="A4" s="1" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="B4" t="s">
-        <v>184</v>
+        <v>187</v>
       </c>
       <c r="C4">
         <v>-0.49</v>
@@ -1101,13 +1137,22 @@
       <c r="M4">
         <v>3</v>
       </c>
-    </row>
-    <row r="5" spans="1:13">
+      <c r="N4">
+        <v>1.23711174845644</v>
+      </c>
+      <c r="O4">
+        <v>0.2466678353455085</v>
+      </c>
+      <c r="P4">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:16">
       <c r="A5" s="1" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="B5" t="s">
-        <v>183</v>
+        <v>186</v>
       </c>
       <c r="C5">
         <v>2.11</v>
@@ -1142,13 +1187,22 @@
       <c r="M5">
         <v>1</v>
       </c>
-    </row>
-    <row r="6" spans="1:13">
+      <c r="N5">
+        <v>-2.114816765168797</v>
+      </c>
+      <c r="O5">
+        <v>0.9549049116538407</v>
+      </c>
+      <c r="P5">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="6" spans="1:16">
       <c r="A6" s="1" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="B6" t="s">
-        <v>184</v>
+        <v>187</v>
       </c>
       <c r="C6">
         <v>0.17</v>
@@ -1183,13 +1237,22 @@
       <c r="M6">
         <v>3</v>
       </c>
-    </row>
-    <row r="7" spans="1:13">
+      <c r="N6">
+        <v>2.374576960373252</v>
+      </c>
+      <c r="O6">
+        <v>0.009157722082276332</v>
+      </c>
+      <c r="P6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:16">
       <c r="A7" s="1" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="B7" t="s">
-        <v>183</v>
+        <v>186</v>
       </c>
       <c r="C7">
         <v>4.26</v>
@@ -1224,13 +1287,22 @@
       <c r="M7">
         <v>2</v>
       </c>
-    </row>
-    <row r="8" spans="1:13">
+      <c r="N7">
+        <v>-1.589117576938125</v>
+      </c>
+      <c r="O7">
+        <v>-1.723940594654304</v>
+      </c>
+      <c r="P7">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="8" spans="1:16">
       <c r="A8" s="1" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="B8" t="s">
-        <v>185</v>
+        <v>188</v>
       </c>
       <c r="C8">
         <v>1.36</v>
@@ -1265,13 +1337,22 @@
       <c r="M8">
         <v>3</v>
       </c>
-    </row>
-    <row r="9" spans="1:13">
+      <c r="N8">
+        <v>2.486553824461864</v>
+      </c>
+      <c r="O8">
+        <v>-0.8570870038434618</v>
+      </c>
+      <c r="P8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:16">
       <c r="A9" s="1" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="B9" t="s">
-        <v>182</v>
+        <v>185</v>
       </c>
       <c r="C9">
         <v>3.14</v>
@@ -1306,13 +1387,22 @@
       <c r="M9">
         <v>2</v>
       </c>
-    </row>
-    <row r="10" spans="1:13">
+      <c r="N9">
+        <v>-0.1219779925040396</v>
+      </c>
+      <c r="O9">
+        <v>-2.609289363650283</v>
+      </c>
+      <c r="P9">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="10" spans="1:16">
       <c r="A10" s="1" t="s">
-        <v>21</v>
+        <v>24</v>
       </c>
       <c r="B10" t="s">
-        <v>185</v>
+        <v>188</v>
       </c>
       <c r="C10">
         <v>1.07</v>
@@ -1347,13 +1437,22 @@
       <c r="M10">
         <v>3</v>
       </c>
-    </row>
-    <row r="11" spans="1:13">
+      <c r="N10">
+        <v>1.073744356574197</v>
+      </c>
+      <c r="O10">
+        <v>1.429868031946236</v>
+      </c>
+      <c r="P10">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="11" spans="1:16">
       <c r="A11" s="1" t="s">
-        <v>22</v>
+        <v>25</v>
       </c>
       <c r="B11" t="s">
-        <v>182</v>
+        <v>185</v>
       </c>
       <c r="C11">
         <v>0.04</v>
@@ -1388,13 +1487,22 @@
       <c r="M11">
         <v>2</v>
       </c>
-    </row>
-    <row r="12" spans="1:13">
+      <c r="N11">
+        <v>0.5177970501459672</v>
+      </c>
+      <c r="O11">
+        <v>-0.03526806183328886</v>
+      </c>
+      <c r="P11">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="12" spans="1:16">
       <c r="A12" s="1" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="B12" t="s">
-        <v>186</v>
+        <v>189</v>
       </c>
       <c r="C12">
         <v>1.75</v>
@@ -1429,13 +1537,22 @@
       <c r="M12">
         <v>3</v>
       </c>
-    </row>
-    <row r="13" spans="1:13">
+      <c r="N12">
+        <v>2.826622072555177</v>
+      </c>
+      <c r="O12">
+        <v>1.152487167634742</v>
+      </c>
+      <c r="P12">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="13" spans="1:16">
       <c r="A13" s="1" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="B13" t="s">
-        <v>184</v>
+        <v>187</v>
       </c>
       <c r="C13">
         <v>0.61</v>
@@ -1470,13 +1587,22 @@
       <c r="M13">
         <v>3</v>
       </c>
-    </row>
-    <row r="14" spans="1:13">
+      <c r="N13">
+        <v>2.698326469749897</v>
+      </c>
+      <c r="O13">
+        <v>0.1106379743758239</v>
+      </c>
+      <c r="P13">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:16">
       <c r="A14" s="1" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="B14" t="s">
-        <v>182</v>
+        <v>185</v>
       </c>
       <c r="C14">
         <v>1.29</v>
@@ -1511,13 +1637,22 @@
       <c r="M14">
         <v>2</v>
       </c>
-    </row>
-    <row r="15" spans="1:13">
+      <c r="N14">
+        <v>-0.6722339071837684</v>
+      </c>
+      <c r="O14">
+        <v>0.1596027130447561</v>
+      </c>
+      <c r="P14">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="15" spans="1:16">
       <c r="A15" s="1" t="s">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="B15" t="s">
-        <v>185</v>
+        <v>188</v>
       </c>
       <c r="C15">
         <v>1.31</v>
@@ -1552,13 +1687,22 @@
       <c r="M15">
         <v>3</v>
       </c>
-    </row>
-    <row r="16" spans="1:13">
+      <c r="N15">
+        <v>2.956253395604683</v>
+      </c>
+      <c r="O15">
+        <v>-0.6576825525323218</v>
+      </c>
+      <c r="P15">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:16">
       <c r="A16" s="1" t="s">
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="B16" t="s">
-        <v>182</v>
+        <v>185</v>
       </c>
       <c r="C16">
         <v>1.19</v>
@@ -1593,13 +1737,22 @@
       <c r="M16">
         <v>1</v>
       </c>
-    </row>
-    <row r="17" spans="1:13">
+      <c r="N16">
+        <v>-2.668250536928177</v>
+      </c>
+      <c r="O16">
+        <v>1.083263565144379</v>
+      </c>
+      <c r="P16">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="17" spans="1:16">
       <c r="A17" s="1" t="s">
-        <v>28</v>
+        <v>31</v>
       </c>
       <c r="B17" t="s">
-        <v>185</v>
+        <v>188</v>
       </c>
       <c r="C17">
         <v>0.27</v>
@@ -1634,13 +1787,22 @@
       <c r="M17">
         <v>3</v>
       </c>
-    </row>
-    <row r="18" spans="1:13">
+      <c r="N17">
+        <v>1.490072988841497</v>
+      </c>
+      <c r="O17">
+        <v>0.1323252082325652</v>
+      </c>
+      <c r="P17">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="18" spans="1:16">
       <c r="A18" s="1" t="s">
-        <v>29</v>
+        <v>32</v>
       </c>
       <c r="B18" t="s">
-        <v>184</v>
+        <v>187</v>
       </c>
       <c r="C18">
         <v>0.68</v>
@@ -1675,13 +1837,22 @@
       <c r="M18">
         <v>3</v>
       </c>
-    </row>
-    <row r="19" spans="1:13">
+      <c r="N18">
+        <v>2.549916646807758</v>
+      </c>
+      <c r="O18">
+        <v>-1.878403733307122</v>
+      </c>
+      <c r="P18">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" spans="1:16">
       <c r="A19" s="1" t="s">
-        <v>30</v>
+        <v>33</v>
       </c>
       <c r="B19" t="s">
-        <v>185</v>
+        <v>188</v>
       </c>
       <c r="C19">
         <v>2.57</v>
@@ -1716,13 +1887,22 @@
       <c r="M19">
         <v>2</v>
       </c>
-    </row>
-    <row r="20" spans="1:13">
+      <c r="N19">
+        <v>-0.5601540678275257</v>
+      </c>
+      <c r="O19">
+        <v>-0.4045085380461237</v>
+      </c>
+      <c r="P19">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="20" spans="1:16">
       <c r="A20" s="1" t="s">
-        <v>31</v>
+        <v>34</v>
       </c>
       <c r="B20" t="s">
-        <v>185</v>
+        <v>188</v>
       </c>
       <c r="C20">
         <v>1.71</v>
@@ -1757,13 +1937,22 @@
       <c r="M20">
         <v>2</v>
       </c>
-    </row>
-    <row r="21" spans="1:13">
+      <c r="N20">
+        <v>-0.2645095456923552</v>
+      </c>
+      <c r="O20">
+        <v>2.02894452597747</v>
+      </c>
+      <c r="P20">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="21" spans="1:16">
       <c r="A21" s="1" t="s">
-        <v>32</v>
+        <v>35</v>
       </c>
       <c r="B21" t="s">
-        <v>184</v>
+        <v>187</v>
       </c>
       <c r="C21">
         <v>-1.09</v>
@@ -1798,13 +1987,22 @@
       <c r="M21">
         <v>2</v>
       </c>
-    </row>
-    <row r="22" spans="1:13">
+      <c r="N21">
+        <v>0.04767303901981641</v>
+      </c>
+      <c r="O21">
+        <v>0.9078026088589561</v>
+      </c>
+      <c r="P21">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="22" spans="1:16">
       <c r="A22" s="1" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="B22" t="s">
-        <v>183</v>
+        <v>186</v>
       </c>
       <c r="C22">
         <v>1.76</v>
@@ -1839,13 +2037,22 @@
       <c r="M22">
         <v>2</v>
       </c>
-    </row>
-    <row r="23" spans="1:13">
+      <c r="N22">
+        <v>0.1194282815915174</v>
+      </c>
+      <c r="O22">
+        <v>-0.219659923562517</v>
+      </c>
+      <c r="P22">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="23" spans="1:16">
       <c r="A23" s="1" t="s">
-        <v>34</v>
+        <v>37</v>
       </c>
       <c r="B23" t="s">
-        <v>185</v>
+        <v>188</v>
       </c>
       <c r="C23">
         <v>0.93</v>
@@ -1880,13 +2087,22 @@
       <c r="M23">
         <v>3</v>
       </c>
-    </row>
-    <row r="24" spans="1:13">
+      <c r="N23">
+        <v>0.8634100196819752</v>
+      </c>
+      <c r="O23">
+        <v>0.3718921722354576</v>
+      </c>
+      <c r="P23">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="24" spans="1:16">
       <c r="A24" s="1" t="s">
-        <v>35</v>
+        <v>38</v>
       </c>
       <c r="B24" t="s">
-        <v>184</v>
+        <v>187</v>
       </c>
       <c r="C24">
         <v>-0.63</v>
@@ -1921,13 +2137,22 @@
       <c r="M24">
         <v>3</v>
       </c>
-    </row>
-    <row r="25" spans="1:13">
+      <c r="N24">
+        <v>1.119840707834355</v>
+      </c>
+      <c r="O24">
+        <v>0.09331135886737493</v>
+      </c>
+      <c r="P24">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="25" spans="1:16">
       <c r="A25" s="1" t="s">
-        <v>36</v>
+        <v>39</v>
       </c>
       <c r="B25" t="s">
-        <v>183</v>
+        <v>186</v>
       </c>
       <c r="C25">
         <v>3.47</v>
@@ -1962,13 +2187,22 @@
       <c r="M25">
         <v>1</v>
       </c>
-    </row>
-    <row r="26" spans="1:13">
+      <c r="N25">
+        <v>-2.902202648331484</v>
+      </c>
+      <c r="O25">
+        <v>0.2772766951117709</v>
+      </c>
+      <c r="P25">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="26" spans="1:16">
       <c r="A26" s="1" t="s">
-        <v>37</v>
+        <v>40</v>
       </c>
       <c r="B26" t="s">
-        <v>184</v>
+        <v>187</v>
       </c>
       <c r="C26">
         <v>-0.03</v>
@@ -2003,13 +2237,22 @@
       <c r="M26">
         <v>3</v>
       </c>
-    </row>
-    <row r="27" spans="1:13">
+      <c r="N26">
+        <v>1.171974536052488</v>
+      </c>
+      <c r="O26">
+        <v>1.423632783575262</v>
+      </c>
+      <c r="P26">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="27" spans="1:16">
       <c r="A27" s="1" t="s">
-        <v>38</v>
+        <v>41</v>
       </c>
       <c r="B27" t="s">
-        <v>183</v>
+        <v>186</v>
       </c>
       <c r="C27">
         <v>3.22</v>
@@ -2044,13 +2287,22 @@
       <c r="M27">
         <v>2</v>
       </c>
-    </row>
-    <row r="28" spans="1:13">
+      <c r="N27">
+        <v>-1.388431971708215</v>
+      </c>
+      <c r="O27">
+        <v>-2.14258605998804</v>
+      </c>
+      <c r="P27">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="28" spans="1:16">
       <c r="A28" s="1" t="s">
-        <v>39</v>
+        <v>42</v>
       </c>
       <c r="B28" t="s">
-        <v>183</v>
+        <v>186</v>
       </c>
       <c r="C28">
         <v>1.31</v>
@@ -2085,13 +2337,22 @@
       <c r="M28">
         <v>2</v>
       </c>
-    </row>
-    <row r="29" spans="1:13">
+      <c r="N28">
+        <v>0.1745598253830776</v>
+      </c>
+      <c r="O28">
+        <v>-1.487162148521828</v>
+      </c>
+      <c r="P28">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="29" spans="1:16">
       <c r="A29" s="1" t="s">
-        <v>40</v>
+        <v>43</v>
       </c>
       <c r="B29" t="s">
-        <v>182</v>
+        <v>185</v>
       </c>
       <c r="C29">
         <v>1.7</v>
@@ -2126,13 +2387,22 @@
       <c r="M29">
         <v>1</v>
       </c>
-    </row>
-    <row r="30" spans="1:13">
+      <c r="N29">
+        <v>-1.580560725809953</v>
+      </c>
+      <c r="O29">
+        <v>0.3832560756558812</v>
+      </c>
+      <c r="P29">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="30" spans="1:16">
       <c r="A30" s="1" t="s">
-        <v>41</v>
+        <v>44</v>
       </c>
       <c r="B30" t="s">
-        <v>183</v>
+        <v>186</v>
       </c>
       <c r="C30">
         <v>3.12</v>
@@ -2167,13 +2437,22 @@
       <c r="M30">
         <v>1</v>
       </c>
-    </row>
-    <row r="31" spans="1:13">
+      <c r="N30">
+        <v>-2.891157031845482</v>
+      </c>
+      <c r="O30">
+        <v>0.4489954735981125</v>
+      </c>
+      <c r="P30">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="31" spans="1:16">
       <c r="A31" s="1" t="s">
-        <v>42</v>
+        <v>45</v>
       </c>
       <c r="B31" t="s">
-        <v>185</v>
+        <v>188</v>
       </c>
       <c r="C31">
         <v>1.15</v>
@@ -2208,13 +2487,22 @@
       <c r="M31">
         <v>3</v>
       </c>
-    </row>
-    <row r="32" spans="1:13">
+      <c r="N31">
+        <v>2.085703052428027</v>
+      </c>
+      <c r="O31">
+        <v>0.1403654016523721</v>
+      </c>
+      <c r="P31">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="32" spans="1:16">
       <c r="A32" s="1" t="s">
-        <v>43</v>
+        <v>46</v>
       </c>
       <c r="B32" t="s">
-        <v>185</v>
+        <v>188</v>
       </c>
       <c r="C32">
         <v>1.17</v>
@@ -2249,13 +2537,22 @@
       <c r="M32">
         <v>3</v>
       </c>
-    </row>
-    <row r="33" spans="1:13">
+      <c r="N32">
+        <v>1.403200280242539</v>
+      </c>
+      <c r="O32">
+        <v>0.8902605472891851</v>
+      </c>
+      <c r="P32">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="33" spans="1:16">
       <c r="A33" s="1" t="s">
-        <v>44</v>
+        <v>47</v>
       </c>
       <c r="B33" t="s">
-        <v>182</v>
+        <v>185</v>
       </c>
       <c r="C33">
         <v>0.68</v>
@@ -2290,13 +2587,22 @@
       <c r="M33">
         <v>3</v>
       </c>
-    </row>
-    <row r="34" spans="1:13">
+      <c r="N33">
+        <v>4.582873653459127</v>
+      </c>
+      <c r="O33">
+        <v>-3.186630084940235</v>
+      </c>
+      <c r="P33">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="34" spans="1:16">
       <c r="A34" s="1" t="s">
-        <v>45</v>
+        <v>48</v>
       </c>
       <c r="B34" t="s">
-        <v>182</v>
+        <v>185</v>
       </c>
       <c r="C34">
         <v>2.34</v>
@@ -2331,13 +2637,22 @@
       <c r="M34">
         <v>3</v>
       </c>
-    </row>
-    <row r="35" spans="1:13">
+      <c r="N34">
+        <v>4.187575663247816</v>
+      </c>
+      <c r="O34">
+        <v>-1.015940844993572</v>
+      </c>
+      <c r="P34">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="35" spans="1:16">
       <c r="A35" s="1" t="s">
-        <v>46</v>
+        <v>49</v>
       </c>
       <c r="B35" t="s">
-        <v>182</v>
+        <v>185</v>
       </c>
       <c r="C35">
         <v>0.33</v>
@@ -2372,13 +2687,22 @@
       <c r="M35">
         <v>3</v>
       </c>
-    </row>
-    <row r="36" spans="1:13">
+      <c r="N35">
+        <v>1.728456868555041</v>
+      </c>
+      <c r="O35">
+        <v>0.3276451385751697</v>
+      </c>
+      <c r="P35">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="36" spans="1:16">
       <c r="A36" s="1" t="s">
-        <v>47</v>
+        <v>50</v>
       </c>
       <c r="B36" t="s">
-        <v>182</v>
+        <v>185</v>
       </c>
       <c r="C36">
         <v>0.5600000000000001</v>
@@ -2413,13 +2737,22 @@
       <c r="M36">
         <v>1</v>
       </c>
-    </row>
-    <row r="37" spans="1:13">
+      <c r="N36">
+        <v>-0.821059994714319</v>
+      </c>
+      <c r="O36">
+        <v>0.6548973604798702</v>
+      </c>
+      <c r="P36">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="37" spans="1:16">
       <c r="A37" s="1" t="s">
-        <v>48</v>
+        <v>51</v>
       </c>
       <c r="B37" t="s">
-        <v>182</v>
+        <v>185</v>
       </c>
       <c r="C37">
         <v>1.09</v>
@@ -2454,13 +2787,22 @@
       <c r="M37">
         <v>3</v>
       </c>
-    </row>
-    <row r="38" spans="1:13">
+      <c r="N37">
+        <v>1.231623805191735</v>
+      </c>
+      <c r="O37">
+        <v>0.3094892030499963</v>
+      </c>
+      <c r="P37">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="38" spans="1:16">
       <c r="A38" s="1" t="s">
-        <v>49</v>
+        <v>52</v>
       </c>
       <c r="B38" t="s">
-        <v>185</v>
+        <v>188</v>
       </c>
       <c r="C38">
         <v>1.18</v>
@@ -2495,13 +2837,22 @@
       <c r="M38">
         <v>2</v>
       </c>
-    </row>
-    <row r="39" spans="1:13">
+      <c r="N38">
+        <v>-0.8331354868731673</v>
+      </c>
+      <c r="O38">
+        <v>0.9518705212533686</v>
+      </c>
+      <c r="P38">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="39" spans="1:16">
       <c r="A39" s="1" t="s">
-        <v>50</v>
+        <v>53</v>
       </c>
       <c r="B39" t="s">
-        <v>183</v>
+        <v>186</v>
       </c>
       <c r="C39">
         <v>3.19</v>
@@ -2536,13 +2887,22 @@
       <c r="M39">
         <v>2</v>
       </c>
-    </row>
-    <row r="40" spans="1:13">
+      <c r="N39">
+        <v>-0.6504530601987876</v>
+      </c>
+      <c r="O39">
+        <v>-1.594345651186888</v>
+      </c>
+      <c r="P39">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="40" spans="1:16">
       <c r="A40" s="1" t="s">
-        <v>51</v>
+        <v>54</v>
       </c>
       <c r="B40" t="s">
-        <v>185</v>
+        <v>188</v>
       </c>
       <c r="C40">
         <v>1.24</v>
@@ -2577,13 +2937,22 @@
       <c r="M40">
         <v>3</v>
       </c>
-    </row>
-    <row r="41" spans="1:13">
+      <c r="N40">
+        <v>0.966752995214375</v>
+      </c>
+      <c r="O40">
+        <v>0.3758133654979715</v>
+      </c>
+      <c r="P40">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="41" spans="1:16">
       <c r="A41" s="1" t="s">
-        <v>52</v>
+        <v>55</v>
       </c>
       <c r="B41" t="s">
-        <v>184</v>
+        <v>187</v>
       </c>
       <c r="C41">
         <v>-0.41</v>
@@ -2618,13 +2987,22 @@
       <c r="M41">
         <v>3</v>
       </c>
-    </row>
-    <row r="42" spans="1:13">
+      <c r="N41">
+        <v>1.760074424316073</v>
+      </c>
+      <c r="O41">
+        <v>0.7446943597405143</v>
+      </c>
+      <c r="P41">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="42" spans="1:16">
       <c r="A42" s="1" t="s">
-        <v>53</v>
+        <v>56</v>
       </c>
       <c r="B42" t="s">
-        <v>185</v>
+        <v>188</v>
       </c>
       <c r="C42">
         <v>0.08</v>
@@ -2659,13 +3037,22 @@
       <c r="M42">
         <v>2</v>
       </c>
-    </row>
-    <row r="43" spans="1:13">
+      <c r="N42">
+        <v>0.3858076828040779</v>
+      </c>
+      <c r="O42">
+        <v>-0.691443875147165</v>
+      </c>
+      <c r="P42">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="43" spans="1:16">
       <c r="A43" s="1" t="s">
-        <v>54</v>
+        <v>57</v>
       </c>
       <c r="B43" t="s">
-        <v>183</v>
+        <v>186</v>
       </c>
       <c r="C43">
         <v>2.75</v>
@@ -2700,13 +3087,22 @@
       <c r="M43">
         <v>1</v>
       </c>
-    </row>
-    <row r="44" spans="1:13">
+      <c r="N43">
+        <v>-2.780858225895268</v>
+      </c>
+      <c r="O43">
+        <v>0.6049232169118214</v>
+      </c>
+      <c r="P43">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="44" spans="1:16">
       <c r="A44" s="1" t="s">
-        <v>55</v>
+        <v>58</v>
       </c>
       <c r="B44" t="s">
-        <v>184</v>
+        <v>187</v>
       </c>
       <c r="C44">
         <v>0.48</v>
@@ -2741,13 +3137,22 @@
       <c r="M44">
         <v>3</v>
       </c>
-    </row>
-    <row r="45" spans="1:13">
+      <c r="N44">
+        <v>3.251810880785572</v>
+      </c>
+      <c r="O44">
+        <v>-0.08611452135536994</v>
+      </c>
+      <c r="P44">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="45" spans="1:16">
       <c r="A45" s="1" t="s">
-        <v>56</v>
+        <v>59</v>
       </c>
       <c r="B45" t="s">
-        <v>183</v>
+        <v>186</v>
       </c>
       <c r="C45">
         <v>1.72</v>
@@ -2782,13 +3187,22 @@
       <c r="M45">
         <v>2</v>
       </c>
-    </row>
-    <row r="46" spans="1:13">
+      <c r="N45">
+        <v>-1.35325525969493</v>
+      </c>
+      <c r="O45">
+        <v>-1.005806099593716</v>
+      </c>
+      <c r="P45">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="46" spans="1:16">
       <c r="A46" s="1" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
       <c r="B46" t="s">
-        <v>185</v>
+        <v>188</v>
       </c>
       <c r="C46">
         <v>0.09</v>
@@ -2823,13 +3237,22 @@
       <c r="M46">
         <v>3</v>
       </c>
-    </row>
-    <row r="47" spans="1:13">
+      <c r="N46">
+        <v>1.617639366730089</v>
+      </c>
+      <c r="O46">
+        <v>-0.7113142187775318</v>
+      </c>
+      <c r="P46">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="47" spans="1:16">
       <c r="A47" s="1" t="s">
-        <v>58</v>
+        <v>61</v>
       </c>
       <c r="B47" t="s">
-        <v>185</v>
+        <v>188</v>
       </c>
       <c r="C47">
         <v>0.46</v>
@@ -2864,13 +3287,22 @@
       <c r="M47">
         <v>2</v>
       </c>
-    </row>
-    <row r="48" spans="1:13">
+      <c r="N47">
+        <v>-0.3381301914238785</v>
+      </c>
+      <c r="O47">
+        <v>0.3390888669090318</v>
+      </c>
+      <c r="P47">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="48" spans="1:16">
       <c r="A48" s="1" t="s">
-        <v>59</v>
+        <v>62</v>
       </c>
       <c r="B48" t="s">
-        <v>184</v>
+        <v>187</v>
       </c>
       <c r="C48">
         <v>0.27</v>
@@ -2905,13 +3337,22 @@
       <c r="M48">
         <v>3</v>
       </c>
-    </row>
-    <row r="49" spans="1:13">
+      <c r="N48">
+        <v>1.560786417013898</v>
+      </c>
+      <c r="O48">
+        <v>1.490307275318904</v>
+      </c>
+      <c r="P48">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="49" spans="1:16">
       <c r="A49" s="1" t="s">
-        <v>60</v>
+        <v>63</v>
       </c>
       <c r="B49" t="s">
-        <v>184</v>
+        <v>187</v>
       </c>
       <c r="C49">
         <v>-0.19</v>
@@ -2946,13 +3387,22 @@
       <c r="M49">
         <v>3</v>
       </c>
-    </row>
-    <row r="50" spans="1:13">
+      <c r="N49">
+        <v>1.844958915753119</v>
+      </c>
+      <c r="O49">
+        <v>0.6972625322540462</v>
+      </c>
+      <c r="P49">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="50" spans="1:16">
       <c r="A50" s="1" t="s">
-        <v>61</v>
+        <v>64</v>
       </c>
       <c r="B50" t="s">
-        <v>183</v>
+        <v>186</v>
       </c>
       <c r="C50">
         <v>0.79</v>
@@ -2987,13 +3437,22 @@
       <c r="M50">
         <v>2</v>
       </c>
-    </row>
-    <row r="51" spans="1:13">
+      <c r="N50">
+        <v>-1.054220515687911</v>
+      </c>
+      <c r="O50">
+        <v>0.04712813540169705</v>
+      </c>
+      <c r="P50">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="51" spans="1:16">
       <c r="A51" s="1" t="s">
-        <v>62</v>
+        <v>65</v>
       </c>
       <c r="B51" t="s">
-        <v>186</v>
+        <v>189</v>
       </c>
       <c r="C51">
         <v>0.49</v>
@@ -3028,13 +3487,22 @@
       <c r="M51">
         <v>2</v>
       </c>
-    </row>
-    <row r="52" spans="1:13">
+      <c r="N51">
+        <v>0.1622517174532253</v>
+      </c>
+      <c r="O51">
+        <v>0.03375680680584689</v>
+      </c>
+      <c r="P51">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="52" spans="1:16">
       <c r="A52" s="1" t="s">
-        <v>63</v>
+        <v>66</v>
       </c>
       <c r="B52" t="s">
-        <v>184</v>
+        <v>187</v>
       </c>
       <c r="C52">
         <v>0.4</v>
@@ -3069,13 +3537,22 @@
       <c r="M52">
         <v>3</v>
       </c>
-    </row>
-    <row r="53" spans="1:13">
+      <c r="N52">
+        <v>2.867098374644427</v>
+      </c>
+      <c r="O52">
+        <v>1.005175290024913</v>
+      </c>
+      <c r="P52">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="53" spans="1:16">
       <c r="A53" s="1" t="s">
-        <v>64</v>
+        <v>67</v>
       </c>
       <c r="B53" t="s">
-        <v>184</v>
+        <v>187</v>
       </c>
       <c r="C53">
         <v>0.48</v>
@@ -3110,13 +3587,22 @@
       <c r="M53">
         <v>3</v>
       </c>
-    </row>
-    <row r="54" spans="1:13">
+      <c r="N53">
+        <v>2.692564839841622</v>
+      </c>
+      <c r="O53">
+        <v>2.562225136470822</v>
+      </c>
+      <c r="P53">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="54" spans="1:16">
       <c r="A54" s="1" t="s">
-        <v>65</v>
+        <v>68</v>
       </c>
       <c r="B54" t="s">
-        <v>184</v>
+        <v>187</v>
       </c>
       <c r="C54">
         <v>0.16</v>
@@ -3151,13 +3637,22 @@
       <c r="M54">
         <v>3</v>
       </c>
-    </row>
-    <row r="55" spans="1:13">
+      <c r="N54">
+        <v>0.6595027712872306</v>
+      </c>
+      <c r="O54">
+        <v>0.8153620106693857</v>
+      </c>
+      <c r="P54">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="55" spans="1:16">
       <c r="A55" s="1" t="s">
-        <v>66</v>
+        <v>69</v>
       </c>
       <c r="B55" t="s">
-        <v>183</v>
+        <v>186</v>
       </c>
       <c r="C55">
         <v>4.02</v>
@@ -3192,13 +3687,22 @@
       <c r="M55">
         <v>2</v>
       </c>
-    </row>
-    <row r="56" spans="1:13">
+      <c r="N55">
+        <v>0.1679313319953225</v>
+      </c>
+      <c r="O55">
+        <v>-1.731292584706383</v>
+      </c>
+      <c r="P55">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="56" spans="1:16">
       <c r="A56" s="1" t="s">
-        <v>67</v>
+        <v>70</v>
       </c>
       <c r="B56" t="s">
-        <v>183</v>
+        <v>186</v>
       </c>
       <c r="C56">
         <v>3.5</v>
@@ -3233,13 +3737,22 @@
       <c r="M56">
         <v>2</v>
       </c>
-    </row>
-    <row r="57" spans="1:13">
+      <c r="N56">
+        <v>-1.067700594946762</v>
+      </c>
+      <c r="O56">
+        <v>-2.513711271888795</v>
+      </c>
+      <c r="P56">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="57" spans="1:16">
       <c r="A57" s="1" t="s">
-        <v>68</v>
+        <v>71</v>
       </c>
       <c r="B57" t="s">
-        <v>183</v>
+        <v>186</v>
       </c>
       <c r="C57">
         <v>2.68</v>
@@ -3274,13 +3787,22 @@
       <c r="M57">
         <v>2</v>
       </c>
-    </row>
-    <row r="58" spans="1:13">
+      <c r="N57">
+        <v>-1.415824205721199</v>
+      </c>
+      <c r="O57">
+        <v>-1.143623896406095</v>
+      </c>
+      <c r="P57">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="58" spans="1:16">
       <c r="A58" s="1" t="s">
-        <v>69</v>
+        <v>72</v>
       </c>
       <c r="B58" t="s">
-        <v>185</v>
+        <v>188</v>
       </c>
       <c r="C58">
         <v>0.54</v>
@@ -3315,13 +3837,22 @@
       <c r="M58">
         <v>2</v>
       </c>
-    </row>
-    <row r="59" spans="1:13">
+      <c r="N58">
+        <v>0.6665222289851778</v>
+      </c>
+      <c r="O58">
+        <v>-1.745825782966462</v>
+      </c>
+      <c r="P58">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="59" spans="1:16">
       <c r="A59" s="1" t="s">
-        <v>70</v>
+        <v>73</v>
       </c>
       <c r="B59" t="s">
-        <v>184</v>
+        <v>187</v>
       </c>
       <c r="C59">
         <v>-0.5</v>
@@ -3356,13 +3887,22 @@
       <c r="M59">
         <v>3</v>
       </c>
-    </row>
-    <row r="60" spans="1:13">
+      <c r="N59">
+        <v>1.949585554785702</v>
+      </c>
+      <c r="O59">
+        <v>2.027349126913045</v>
+      </c>
+      <c r="P59">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="60" spans="1:16">
       <c r="A60" s="1" t="s">
-        <v>71</v>
+        <v>74</v>
       </c>
       <c r="B60" t="s">
-        <v>185</v>
+        <v>188</v>
       </c>
       <c r="C60">
         <v>2.35</v>
@@ -3397,13 +3937,22 @@
       <c r="M60">
         <v>2</v>
       </c>
-    </row>
-    <row r="61" spans="1:13">
+      <c r="N60">
+        <v>-1.527730856160604</v>
+      </c>
+      <c r="O60">
+        <v>-0.2688878075154326</v>
+      </c>
+      <c r="P60">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="61" spans="1:16">
       <c r="A61" s="1" t="s">
-        <v>72</v>
+        <v>75</v>
       </c>
       <c r="B61" t="s">
-        <v>183</v>
+        <v>186</v>
       </c>
       <c r="C61">
         <v>2.68</v>
@@ -3438,13 +3987,22 @@
       <c r="M61">
         <v>1</v>
       </c>
-    </row>
-    <row r="62" spans="1:13">
+      <c r="N61">
+        <v>-2.33903581026106</v>
+      </c>
+      <c r="O61">
+        <v>-0.5709052565843564</v>
+      </c>
+      <c r="P61">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="62" spans="1:16">
       <c r="A62" s="1" t="s">
-        <v>73</v>
+        <v>76</v>
       </c>
       <c r="B62" t="s">
-        <v>183</v>
+        <v>186</v>
       </c>
       <c r="C62">
         <v>2.95</v>
@@ -3479,13 +4037,22 @@
       <c r="M62">
         <v>2</v>
       </c>
-    </row>
-    <row r="63" spans="1:13">
+      <c r="N62">
+        <v>-2.046093232551849</v>
+      </c>
+      <c r="O62">
+        <v>-1.31480569097148</v>
+      </c>
+      <c r="P62">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="63" spans="1:16">
       <c r="A63" s="1" t="s">
-        <v>74</v>
+        <v>77</v>
       </c>
       <c r="B63" t="s">
-        <v>185</v>
+        <v>188</v>
       </c>
       <c r="C63">
         <v>0.39</v>
@@ -3520,13 +4087,22 @@
       <c r="M63">
         <v>2</v>
       </c>
-    </row>
-    <row r="64" spans="1:13">
+      <c r="N63">
+        <v>-0.06661315170382999</v>
+      </c>
+      <c r="O63">
+        <v>0.1598980749966497</v>
+      </c>
+      <c r="P63">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="64" spans="1:16">
       <c r="A64" s="1" t="s">
-        <v>75</v>
+        <v>78</v>
       </c>
       <c r="B64" t="s">
-        <v>182</v>
+        <v>185</v>
       </c>
       <c r="C64">
         <v>-0.38</v>
@@ -3561,13 +4137,22 @@
       <c r="M64">
         <v>2</v>
       </c>
-    </row>
-    <row r="65" spans="1:13">
+      <c r="N64">
+        <v>-0.09489274267863565</v>
+      </c>
+      <c r="O64">
+        <v>-0.1705580292960508</v>
+      </c>
+      <c r="P64">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="65" spans="1:16">
       <c r="A65" s="1" t="s">
-        <v>76</v>
+        <v>79</v>
       </c>
       <c r="B65" t="s">
-        <v>185</v>
+        <v>188</v>
       </c>
       <c r="C65">
         <v>1.57</v>
@@ -3602,13 +4187,22 @@
       <c r="M65">
         <v>2</v>
       </c>
-    </row>
-    <row r="66" spans="1:13">
+      <c r="N65">
+        <v>-1.663095372376173</v>
+      </c>
+      <c r="O65">
+        <v>-1.260621083701493</v>
+      </c>
+      <c r="P65">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="66" spans="1:16">
       <c r="A66" s="1" t="s">
-        <v>77</v>
+        <v>80</v>
       </c>
       <c r="B66" t="s">
-        <v>185</v>
+        <v>188</v>
       </c>
       <c r="C66">
         <v>2.08</v>
@@ -3643,13 +4237,22 @@
       <c r="M66">
         <v>2</v>
       </c>
-    </row>
-    <row r="67" spans="1:13">
+      <c r="N66">
+        <v>-1.137290023422126</v>
+      </c>
+      <c r="O66">
+        <v>-0.4946925486697403</v>
+      </c>
+      <c r="P66">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="67" spans="1:16">
       <c r="A67" s="1" t="s">
-        <v>78</v>
+        <v>81</v>
       </c>
       <c r="B67" t="s">
-        <v>184</v>
+        <v>187</v>
       </c>
       <c r="C67">
         <v>-0.29</v>
@@ -3684,13 +4287,22 @@
       <c r="M67">
         <v>3</v>
       </c>
-    </row>
-    <row r="68" spans="1:13">
+      <c r="N67">
+        <v>1.332337469712288</v>
+      </c>
+      <c r="O67">
+        <v>2.311805423173221</v>
+      </c>
+      <c r="P67">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="68" spans="1:16">
       <c r="A68" s="1" t="s">
-        <v>79</v>
+        <v>82</v>
       </c>
       <c r="B68" t="s">
-        <v>182</v>
+        <v>185</v>
       </c>
       <c r="C68">
         <v>1.31</v>
@@ -3725,13 +4337,22 @@
       <c r="M68">
         <v>1</v>
       </c>
-    </row>
-    <row r="69" spans="1:13">
+      <c r="N68">
+        <v>-4.215141019714405</v>
+      </c>
+      <c r="O68">
+        <v>1.781325722311074</v>
+      </c>
+      <c r="P68">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="69" spans="1:16">
       <c r="A69" s="1" t="s">
-        <v>80</v>
+        <v>83</v>
       </c>
       <c r="B69" t="s">
-        <v>182</v>
+        <v>185</v>
       </c>
       <c r="C69">
         <v>1.39</v>
@@ -3766,13 +4387,22 @@
       <c r="M69">
         <v>1</v>
       </c>
-    </row>
-    <row r="70" spans="1:13">
+      <c r="N69">
+        <v>-1.721153986362914</v>
+      </c>
+      <c r="O69">
+        <v>0.8261149605676796</v>
+      </c>
+      <c r="P69">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="70" spans="1:16">
       <c r="A70" s="1" t="s">
-        <v>81</v>
+        <v>84</v>
       </c>
       <c r="B70" t="s">
-        <v>182</v>
+        <v>185</v>
       </c>
       <c r="C70">
         <v>1.31</v>
@@ -3807,13 +4437,22 @@
       <c r="M70">
         <v>2</v>
       </c>
-    </row>
-    <row r="71" spans="1:13">
+      <c r="N70">
+        <v>-1.405257666849225</v>
+      </c>
+      <c r="O70">
+        <v>-1.194682018607679</v>
+      </c>
+      <c r="P70">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="71" spans="1:16">
       <c r="A71" s="1" t="s">
-        <v>82</v>
+        <v>85</v>
       </c>
       <c r="B71" t="s">
-        <v>182</v>
+        <v>185</v>
       </c>
       <c r="C71">
         <v>3.45</v>
@@ -3848,13 +4487,22 @@
       <c r="M71">
         <v>2</v>
       </c>
-    </row>
-    <row r="72" spans="1:13">
+      <c r="N71">
+        <v>-2.314101276316944</v>
+      </c>
+      <c r="O71">
+        <v>-1.540848408406213</v>
+      </c>
+      <c r="P71">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="72" spans="1:16">
       <c r="A72" s="1" t="s">
-        <v>83</v>
+        <v>86</v>
       </c>
       <c r="B72" t="s">
-        <v>184</v>
+        <v>187</v>
       </c>
       <c r="C72">
         <v>0.99</v>
@@ -3889,13 +4537,22 @@
       <c r="M72">
         <v>3</v>
       </c>
-    </row>
-    <row r="73" spans="1:13">
+      <c r="N72">
+        <v>3.233010929132727</v>
+      </c>
+      <c r="O72">
+        <v>-0.4227275885669363</v>
+      </c>
+      <c r="P72">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="73" spans="1:16">
       <c r="A73" s="1" t="s">
-        <v>84</v>
+        <v>87</v>
       </c>
       <c r="B73" t="s">
-        <v>184</v>
+        <v>187</v>
       </c>
       <c r="C73">
         <v>0.96</v>
@@ -3930,13 +4587,22 @@
       <c r="M73">
         <v>3</v>
       </c>
-    </row>
-    <row r="74" spans="1:13">
+      <c r="N73">
+        <v>3.809891268781054</v>
+      </c>
+      <c r="O73">
+        <v>0.7977944218967901</v>
+      </c>
+      <c r="P73">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="74" spans="1:16">
       <c r="A74" s="1" t="s">
-        <v>85</v>
+        <v>88</v>
       </c>
       <c r="B74" t="s">
-        <v>182</v>
+        <v>185</v>
       </c>
       <c r="C74">
         <v>2.04</v>
@@ -3971,13 +4637,22 @@
       <c r="M74">
         <v>3</v>
       </c>
-    </row>
-    <row r="75" spans="1:13">
+      <c r="N74">
+        <v>0.8979008120174493</v>
+      </c>
+      <c r="O74">
+        <v>0.7481632306091577</v>
+      </c>
+      <c r="P74">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="75" spans="1:16">
       <c r="A75" s="1" t="s">
-        <v>86</v>
+        <v>89</v>
       </c>
       <c r="B75" t="s">
-        <v>184</v>
+        <v>187</v>
       </c>
       <c r="C75">
         <v>0.33</v>
@@ -4012,13 +4687,22 @@
       <c r="M75">
         <v>3</v>
       </c>
-    </row>
-    <row r="76" spans="1:13">
+      <c r="N75">
+        <v>1.676589959742453</v>
+      </c>
+      <c r="O75">
+        <v>1.297541915053992</v>
+      </c>
+      <c r="P75">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="76" spans="1:16">
       <c r="A76" s="1" t="s">
-        <v>87</v>
+        <v>90</v>
       </c>
       <c r="B76" t="s">
-        <v>185</v>
+        <v>188</v>
       </c>
       <c r="C76">
         <v>0.55</v>
@@ -4053,13 +4737,22 @@
       <c r="M76">
         <v>2</v>
       </c>
-    </row>
-    <row r="77" spans="1:13">
+      <c r="N76">
+        <v>0.4942683749356915</v>
+      </c>
+      <c r="O76">
+        <v>-0.21916821043059</v>
+      </c>
+      <c r="P76">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="77" spans="1:16">
       <c r="A77" s="1" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
       <c r="B77" t="s">
-        <v>182</v>
+        <v>185</v>
       </c>
       <c r="C77">
         <v>5.64</v>
@@ -4094,13 +4787,22 @@
       <c r="M77">
         <v>2</v>
       </c>
-    </row>
-    <row r="78" spans="1:13">
+      <c r="N77">
+        <v>-1.441317317900737</v>
+      </c>
+      <c r="O77">
+        <v>-1.878220989995969</v>
+      </c>
+      <c r="P77">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="78" spans="1:16">
       <c r="A78" s="1" t="s">
-        <v>89</v>
+        <v>92</v>
       </c>
       <c r="B78" t="s">
-        <v>182</v>
+        <v>185</v>
       </c>
       <c r="C78">
         <v>1.51</v>
@@ -4135,13 +4837,22 @@
       <c r="M78">
         <v>3</v>
       </c>
-    </row>
-    <row r="79" spans="1:13">
+      <c r="N78">
+        <v>1.127787243384577</v>
+      </c>
+      <c r="O78">
+        <v>0.08264019195453172</v>
+      </c>
+      <c r="P78">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="79" spans="1:16">
       <c r="A79" s="1" t="s">
-        <v>90</v>
+        <v>93</v>
       </c>
       <c r="B79" t="s">
-        <v>183</v>
+        <v>186</v>
       </c>
       <c r="C79">
         <v>2.98</v>
@@ -4176,13 +4887,22 @@
       <c r="M79">
         <v>1</v>
       </c>
-    </row>
-    <row r="80" spans="1:13">
+      <c r="N79">
+        <v>-2.940393756350792</v>
+      </c>
+      <c r="O79">
+        <v>0.9462739288685328</v>
+      </c>
+      <c r="P79">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="80" spans="1:16">
       <c r="A80" s="1" t="s">
-        <v>91</v>
+        <v>94</v>
       </c>
       <c r="B80" t="s">
-        <v>182</v>
+        <v>185</v>
       </c>
       <c r="C80">
         <v>1.94</v>
@@ -4217,13 +4937,22 @@
       <c r="M80">
         <v>2</v>
       </c>
-    </row>
-    <row r="81" spans="1:13">
+      <c r="N80">
+        <v>-0.8444323358045106</v>
+      </c>
+      <c r="O80">
+        <v>-0.3891473137742472</v>
+      </c>
+      <c r="P80">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="81" spans="1:16">
       <c r="A81" s="1" t="s">
-        <v>92</v>
+        <v>95</v>
       </c>
       <c r="B81" t="s">
-        <v>186</v>
+        <v>189</v>
       </c>
       <c r="C81">
         <v>1.83</v>
@@ -4258,13 +4987,22 @@
       <c r="M81">
         <v>2</v>
       </c>
-    </row>
-    <row r="82" spans="1:13">
+      <c r="N81">
+        <v>0.4682589498859397</v>
+      </c>
+      <c r="O81">
+        <v>-0.5677848134676895</v>
+      </c>
+      <c r="P81">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="82" spans="1:16">
       <c r="A82" s="1" t="s">
-        <v>93</v>
+        <v>96</v>
       </c>
       <c r="B82" t="s">
-        <v>182</v>
+        <v>185</v>
       </c>
       <c r="C82">
         <v>6.2</v>
@@ -4299,13 +5037,22 @@
       <c r="M82">
         <v>2</v>
       </c>
-    </row>
-    <row r="83" spans="1:13">
+      <c r="N82">
+        <v>0.6315912275171686</v>
+      </c>
+      <c r="O82">
+        <v>-2.109775265709898</v>
+      </c>
+      <c r="P82">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="83" spans="1:16">
       <c r="A83" s="1" t="s">
-        <v>94</v>
+        <v>97</v>
       </c>
       <c r="B83" t="s">
-        <v>183</v>
+        <v>186</v>
       </c>
       <c r="C83">
         <v>0.53</v>
@@ -4340,13 +5087,22 @@
       <c r="M83">
         <v>2</v>
       </c>
-    </row>
-    <row r="84" spans="1:13">
+      <c r="N83">
+        <v>-0.7321107015493511</v>
+      </c>
+      <c r="O83">
+        <v>-0.6741921217934651</v>
+      </c>
+      <c r="P83">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="84" spans="1:16">
       <c r="A84" s="1" t="s">
-        <v>95</v>
+        <v>98</v>
       </c>
       <c r="B84" t="s">
-        <v>184</v>
+        <v>187</v>
       </c>
       <c r="C84">
         <v>-1.12</v>
@@ -4381,13 +5137,22 @@
       <c r="M84">
         <v>3</v>
       </c>
-    </row>
-    <row r="85" spans="1:13">
+      <c r="N84">
+        <v>2.191302444158779</v>
+      </c>
+      <c r="O84">
+        <v>0.2030106688037952</v>
+      </c>
+      <c r="P84">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="85" spans="1:16">
       <c r="A85" s="1" t="s">
-        <v>96</v>
+        <v>99</v>
       </c>
       <c r="B85" t="s">
-        <v>182</v>
+        <v>185</v>
       </c>
       <c r="C85">
         <v>4.3</v>
@@ -4422,13 +5187,22 @@
       <c r="M85">
         <v>1</v>
       </c>
-    </row>
-    <row r="86" spans="1:13">
+      <c r="N85">
+        <v>-1.975405218846225</v>
+      </c>
+      <c r="O85">
+        <v>-0.5987477341880248</v>
+      </c>
+      <c r="P85">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="86" spans="1:16">
       <c r="A86" s="1" t="s">
-        <v>97</v>
+        <v>100</v>
       </c>
       <c r="B86" t="s">
-        <v>183</v>
+        <v>186</v>
       </c>
       <c r="C86">
         <v>3.58</v>
@@ -4463,13 +5237,22 @@
       <c r="M86">
         <v>2</v>
       </c>
-    </row>
-    <row r="87" spans="1:13">
+      <c r="N86">
+        <v>-1.631348833586898</v>
+      </c>
+      <c r="O86">
+        <v>-1.883325772179616</v>
+      </c>
+      <c r="P86">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="87" spans="1:16">
       <c r="A87" s="1" t="s">
-        <v>98</v>
+        <v>101</v>
       </c>
       <c r="B87" t="s">
-        <v>184</v>
+        <v>187</v>
       </c>
       <c r="C87">
         <v>-1.27</v>
@@ -4504,13 +5287,22 @@
       <c r="M87">
         <v>3</v>
       </c>
-    </row>
-    <row r="88" spans="1:13">
+      <c r="N87">
+        <v>2.703898311725352</v>
+      </c>
+      <c r="O87">
+        <v>0.8716444945647417</v>
+      </c>
+      <c r="P87">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="88" spans="1:16">
       <c r="A88" s="1" t="s">
-        <v>99</v>
+        <v>102</v>
       </c>
       <c r="B88" t="s">
-        <v>184</v>
+        <v>187</v>
       </c>
       <c r="C88">
         <v>2.46</v>
@@ -4545,13 +5337,22 @@
       <c r="M88">
         <v>3</v>
       </c>
-    </row>
-    <row r="89" spans="1:13">
+      <c r="N88">
+        <v>3.907550465060897</v>
+      </c>
+      <c r="O88">
+        <v>-0.8496957124830927</v>
+      </c>
+      <c r="P88">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="89" spans="1:16">
       <c r="A89" s="1" t="s">
-        <v>100</v>
+        <v>103</v>
       </c>
       <c r="B89" t="s">
-        <v>184</v>
+        <v>187</v>
       </c>
       <c r="C89">
         <v>0.08</v>
@@ -4586,13 +5387,22 @@
       <c r="M89">
         <v>2</v>
       </c>
-    </row>
-    <row r="90" spans="1:13">
+      <c r="N89">
+        <v>0.3281202388129153</v>
+      </c>
+      <c r="O89">
+        <v>-0.5379633756502311</v>
+      </c>
+      <c r="P89">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="90" spans="1:16">
       <c r="A90" s="1" t="s">
-        <v>101</v>
+        <v>104</v>
       </c>
       <c r="B90" t="s">
-        <v>183</v>
+        <v>186</v>
       </c>
       <c r="C90">
         <v>3.16</v>
@@ -4627,13 +5437,22 @@
       <c r="M90">
         <v>1</v>
       </c>
-    </row>
-    <row r="91" spans="1:13">
+      <c r="N90">
+        <v>-2.520186936473993</v>
+      </c>
+      <c r="O90">
+        <v>0.0502786683163209</v>
+      </c>
+      <c r="P90">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="91" spans="1:16">
       <c r="A91" s="1" t="s">
-        <v>102</v>
+        <v>105</v>
       </c>
       <c r="B91" t="s">
-        <v>182</v>
+        <v>185</v>
       </c>
       <c r="C91">
         <v>1.64</v>
@@ -4668,13 +5487,22 @@
       <c r="M91">
         <v>3</v>
       </c>
-    </row>
-    <row r="92" spans="1:13">
+      <c r="N91">
+        <v>0.8866808434193805</v>
+      </c>
+      <c r="O91">
+        <v>2.192146546194619</v>
+      </c>
+      <c r="P91">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="92" spans="1:16">
       <c r="A92" s="1" t="s">
-        <v>103</v>
+        <v>106</v>
       </c>
       <c r="B92" t="s">
-        <v>183</v>
+        <v>186</v>
       </c>
       <c r="C92">
         <v>3.24</v>
@@ -4709,13 +5537,22 @@
       <c r="M92">
         <v>1</v>
       </c>
-    </row>
-    <row r="93" spans="1:13">
+      <c r="N92">
+        <v>-2.546537935680068</v>
+      </c>
+      <c r="O92">
+        <v>0.9448792103585076</v>
+      </c>
+      <c r="P92">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="93" spans="1:16">
       <c r="A93" s="1" t="s">
-        <v>104</v>
+        <v>107</v>
       </c>
       <c r="B93" t="s">
-        <v>182</v>
+        <v>185</v>
       </c>
       <c r="C93">
         <v>4.81</v>
@@ -4750,13 +5587,22 @@
       <c r="M93">
         <v>2</v>
       </c>
-    </row>
-    <row r="94" spans="1:13">
+      <c r="N93">
+        <v>-0.5796046346578471</v>
+      </c>
+      <c r="O93">
+        <v>-1.80562657486473</v>
+      </c>
+      <c r="P93">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="94" spans="1:16">
       <c r="A94" s="1" t="s">
-        <v>105</v>
+        <v>108</v>
       </c>
       <c r="B94" t="s">
-        <v>183</v>
+        <v>186</v>
       </c>
       <c r="C94">
         <v>3.56</v>
@@ -4791,13 +5637,22 @@
       <c r="M94">
         <v>1</v>
       </c>
-    </row>
-    <row r="95" spans="1:13">
+      <c r="N94">
+        <v>-2.456350041610883</v>
+      </c>
+      <c r="O94">
+        <v>-0.1984555294680149</v>
+      </c>
+      <c r="P94">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="95" spans="1:16">
       <c r="A95" s="1" t="s">
-        <v>106</v>
+        <v>109</v>
       </c>
       <c r="B95" t="s">
-        <v>184</v>
+        <v>187</v>
       </c>
       <c r="C95">
         <v>0.74</v>
@@ -4832,13 +5687,22 @@
       <c r="M95">
         <v>3</v>
       </c>
-    </row>
-    <row r="96" spans="1:13">
+      <c r="N95">
+        <v>2.378466844517986</v>
+      </c>
+      <c r="O95">
+        <v>-0.2463356819450533</v>
+      </c>
+      <c r="P95">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="96" spans="1:16">
       <c r="A96" s="1" t="s">
-        <v>107</v>
+        <v>110</v>
       </c>
       <c r="B96" t="s">
-        <v>183</v>
+        <v>186</v>
       </c>
       <c r="C96">
         <v>1.42</v>
@@ -4873,13 +5737,22 @@
       <c r="M96">
         <v>2</v>
       </c>
-    </row>
-    <row r="97" spans="1:13">
+      <c r="N96">
+        <v>-0.9417386103220493</v>
+      </c>
+      <c r="O96">
+        <v>0.1550051882777176</v>
+      </c>
+      <c r="P96">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="97" spans="1:16">
       <c r="A97" s="1" t="s">
-        <v>108</v>
+        <v>111</v>
       </c>
       <c r="B97" t="s">
-        <v>183</v>
+        <v>186</v>
       </c>
       <c r="C97">
         <v>0.25</v>
@@ -4914,13 +5787,22 @@
       <c r="M97">
         <v>3</v>
       </c>
-    </row>
-    <row r="98" spans="1:13">
+      <c r="N97">
+        <v>0.9476125331007231</v>
+      </c>
+      <c r="O97">
+        <v>0.08183985669781121</v>
+      </c>
+      <c r="P97">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="98" spans="1:16">
       <c r="A98" s="1" t="s">
-        <v>109</v>
+        <v>112</v>
       </c>
       <c r="B98" t="s">
-        <v>183</v>
+        <v>186</v>
       </c>
       <c r="C98">
         <v>3.37</v>
@@ -4955,13 +5837,22 @@
       <c r="M98">
         <v>2</v>
       </c>
-    </row>
-    <row r="99" spans="1:13">
+      <c r="N98">
+        <v>-1.136704804996464</v>
+      </c>
+      <c r="O98">
+        <v>-1.151064215997423</v>
+      </c>
+      <c r="P98">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="99" spans="1:16">
       <c r="A99" s="1" t="s">
-        <v>110</v>
+        <v>113</v>
       </c>
       <c r="B99" t="s">
-        <v>185</v>
+        <v>188</v>
       </c>
       <c r="C99">
         <v>1.43</v>
@@ -4996,13 +5887,22 @@
       <c r="M99">
         <v>2</v>
       </c>
-    </row>
-    <row r="100" spans="1:13">
+      <c r="N99">
+        <v>-0.3180309088225146</v>
+      </c>
+      <c r="O99">
+        <v>0.5713746364890112</v>
+      </c>
+      <c r="P99">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="100" spans="1:16">
       <c r="A100" s="1" t="s">
-        <v>111</v>
+        <v>114</v>
       </c>
       <c r="B100" t="s">
-        <v>182</v>
+        <v>185</v>
       </c>
       <c r="C100">
         <v>2</v>
@@ -5037,13 +5937,22 @@
       <c r="M100">
         <v>3</v>
       </c>
-    </row>
-    <row r="101" spans="1:13">
+      <c r="N100">
+        <v>1.845190267584877</v>
+      </c>
+      <c r="O100">
+        <v>-0.4883088139334144</v>
+      </c>
+      <c r="P100">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="101" spans="1:16">
       <c r="A101" s="1" t="s">
-        <v>112</v>
+        <v>115</v>
       </c>
       <c r="B101" t="s">
-        <v>184</v>
+        <v>187</v>
       </c>
       <c r="C101">
         <v>0.13</v>
@@ -5078,13 +5987,22 @@
       <c r="M101">
         <v>3</v>
       </c>
-    </row>
-    <row r="102" spans="1:13">
+      <c r="N101">
+        <v>1.827381922225326</v>
+      </c>
+      <c r="O101">
+        <v>0.1710956640859014</v>
+      </c>
+      <c r="P101">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="102" spans="1:16">
       <c r="A102" s="1" t="s">
-        <v>113</v>
+        <v>116</v>
       </c>
       <c r="B102" t="s">
-        <v>183</v>
+        <v>186</v>
       </c>
       <c r="C102">
         <v>3.22</v>
@@ -5119,13 +6037,22 @@
       <c r="M102">
         <v>1</v>
       </c>
-    </row>
-    <row r="103" spans="1:13">
+      <c r="N102">
+        <v>-2.264008473752768</v>
+      </c>
+      <c r="O102">
+        <v>-0.1109213906863095</v>
+      </c>
+      <c r="P102">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="103" spans="1:16">
       <c r="A103" s="1" t="s">
-        <v>114</v>
+        <v>117</v>
       </c>
       <c r="B103" t="s">
-        <v>182</v>
+        <v>185</v>
       </c>
       <c r="C103">
         <v>0.76</v>
@@ -5160,13 +6087,22 @@
       <c r="M103">
         <v>2</v>
       </c>
-    </row>
-    <row r="104" spans="1:13">
+      <c r="N103">
+        <v>-0.5928194637564239</v>
+      </c>
+      <c r="O103">
+        <v>0.9453318152580834</v>
+      </c>
+      <c r="P103">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="104" spans="1:16">
       <c r="A104" s="1" t="s">
-        <v>115</v>
+        <v>118</v>
       </c>
       <c r="B104" t="s">
-        <v>183</v>
+        <v>186</v>
       </c>
       <c r="C104">
         <v>1.97</v>
@@ -5201,13 +6137,22 @@
       <c r="M104">
         <v>2</v>
       </c>
-    </row>
-    <row r="105" spans="1:13">
+      <c r="N104">
+        <v>-0.06449091935328302</v>
+      </c>
+      <c r="O104">
+        <v>-1.394328180687982</v>
+      </c>
+      <c r="P104">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="105" spans="1:16">
       <c r="A105" s="1" t="s">
-        <v>116</v>
+        <v>119</v>
       </c>
       <c r="B105" t="s">
-        <v>185</v>
+        <v>188</v>
       </c>
       <c r="C105">
         <v>1.42</v>
@@ -5242,13 +6187,22 @@
       <c r="M105">
         <v>2</v>
       </c>
-    </row>
-    <row r="106" spans="1:13">
+      <c r="N105">
+        <v>-0.9271542863218917</v>
+      </c>
+      <c r="O105">
+        <v>-0.2553215729059843</v>
+      </c>
+      <c r="P105">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="106" spans="1:16">
       <c r="A106" s="1" t="s">
-        <v>117</v>
+        <v>120</v>
       </c>
       <c r="B106" t="s">
-        <v>183</v>
+        <v>186</v>
       </c>
       <c r="C106">
         <v>4.71</v>
@@ -5283,13 +6237,22 @@
       <c r="M106">
         <v>1</v>
       </c>
-    </row>
-    <row r="107" spans="1:13">
+      <c r="N106">
+        <v>-3.542033448399215</v>
+      </c>
+      <c r="O106">
+        <v>0.008279864243136009</v>
+      </c>
+      <c r="P106">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="107" spans="1:16">
       <c r="A107" s="1" t="s">
-        <v>118</v>
+        <v>121</v>
       </c>
       <c r="B107" t="s">
-        <v>183</v>
+        <v>186</v>
       </c>
       <c r="C107">
         <v>3.04</v>
@@ -5324,13 +6287,22 @@
       <c r="M107">
         <v>1</v>
       </c>
-    </row>
-    <row r="108" spans="1:13">
+      <c r="N107">
+        <v>-3.721062641338247</v>
+      </c>
+      <c r="O107">
+        <v>0.7278417407927463</v>
+      </c>
+      <c r="P107">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="108" spans="1:16">
       <c r="A108" s="1" t="s">
-        <v>119</v>
+        <v>122</v>
       </c>
       <c r="B108" t="s">
-        <v>184</v>
+        <v>187</v>
       </c>
       <c r="C108">
         <v>1.22</v>
@@ -5365,13 +6337,22 @@
       <c r="M108">
         <v>3</v>
       </c>
-    </row>
-    <row r="109" spans="1:13">
+      <c r="N108">
+        <v>2.648142771181356</v>
+      </c>
+      <c r="O108">
+        <v>0.6136614557017053</v>
+      </c>
+      <c r="P108">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="109" spans="1:16">
       <c r="A109" s="1" t="s">
-        <v>120</v>
+        <v>123</v>
       </c>
       <c r="B109" t="s">
-        <v>186</v>
+        <v>189</v>
       </c>
       <c r="C109">
         <v>1.39</v>
@@ -5406,13 +6387,22 @@
       <c r="M109">
         <v>3</v>
       </c>
-    </row>
-    <row r="110" spans="1:13">
+      <c r="N109">
+        <v>1.632198370419451</v>
+      </c>
+      <c r="O109">
+        <v>-0.7889788145427232</v>
+      </c>
+      <c r="P109">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="110" spans="1:16">
       <c r="A110" s="1" t="s">
-        <v>121</v>
+        <v>124</v>
       </c>
       <c r="B110" t="s">
-        <v>186</v>
+        <v>189</v>
       </c>
       <c r="C110">
         <v>1.11</v>
@@ -5447,13 +6437,22 @@
       <c r="M110">
         <v>3</v>
       </c>
-    </row>
-    <row r="111" spans="1:13">
+      <c r="N110">
+        <v>2.154962747402586</v>
+      </c>
+      <c r="O110">
+        <v>0.6323001275939779</v>
+      </c>
+      <c r="P110">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="111" spans="1:16">
       <c r="A111" s="1" t="s">
-        <v>122</v>
+        <v>125</v>
       </c>
       <c r="B111" t="s">
-        <v>182</v>
+        <v>185</v>
       </c>
       <c r="C111">
         <v>0.47</v>
@@ -5488,13 +6487,22 @@
       <c r="M111">
         <v>1</v>
       </c>
-    </row>
-    <row r="112" spans="1:13">
+      <c r="N111">
+        <v>-2.683502232290432</v>
+      </c>
+      <c r="O111">
+        <v>1.375323064187996</v>
+      </c>
+      <c r="P111">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="112" spans="1:16">
       <c r="A112" s="1" t="s">
-        <v>123</v>
+        <v>126</v>
       </c>
       <c r="B112" t="s">
-        <v>182</v>
+        <v>185</v>
       </c>
       <c r="C112">
         <v>7.56</v>
@@ -5529,13 +6537,22 @@
       <c r="M112">
         <v>2</v>
       </c>
-    </row>
-    <row r="113" spans="1:13">
+      <c r="N112">
+        <v>0.1103633206185996</v>
+      </c>
+      <c r="O112">
+        <v>-2.642792950682062</v>
+      </c>
+      <c r="P112">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="113" spans="1:16">
       <c r="A113" s="1" t="s">
-        <v>124</v>
+        <v>127</v>
       </c>
       <c r="B113" t="s">
-        <v>183</v>
+        <v>186</v>
       </c>
       <c r="C113">
         <v>3.96</v>
@@ -5570,13 +6587,22 @@
       <c r="M113">
         <v>1</v>
       </c>
-    </row>
-    <row r="114" spans="1:13">
+      <c r="N113">
+        <v>-3.054435707477832</v>
+      </c>
+      <c r="O113">
+        <v>0.3367869885556987</v>
+      </c>
+      <c r="P113">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="114" spans="1:16">
       <c r="A114" s="1" t="s">
-        <v>125</v>
+        <v>128</v>
       </c>
       <c r="B114" t="s">
-        <v>182</v>
+        <v>185</v>
       </c>
       <c r="C114">
         <v>2.39</v>
@@ -5611,13 +6637,22 @@
       <c r="M114">
         <v>1</v>
       </c>
-    </row>
-    <row r="115" spans="1:13">
+      <c r="N114">
+        <v>-2.504535444476235</v>
+      </c>
+      <c r="O114">
+        <v>1.229277472821156</v>
+      </c>
+      <c r="P114">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="115" spans="1:16">
       <c r="A115" s="1" t="s">
-        <v>126</v>
+        <v>129</v>
       </c>
       <c r="B115" t="s">
-        <v>185</v>
+        <v>188</v>
       </c>
       <c r="C115">
         <v>1.89</v>
@@ -5652,13 +6687,22 @@
       <c r="M115">
         <v>3</v>
       </c>
-    </row>
-    <row r="116" spans="1:13">
+      <c r="N115">
+        <v>0.7926376806236393</v>
+      </c>
+      <c r="O115">
+        <v>0.4582744216679233</v>
+      </c>
+      <c r="P115">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="116" spans="1:16">
       <c r="A116" s="1" t="s">
-        <v>127</v>
+        <v>130</v>
       </c>
       <c r="B116" t="s">
-        <v>185</v>
+        <v>188</v>
       </c>
       <c r="C116">
         <v>1.45</v>
@@ -5693,13 +6737,22 @@
       <c r="M116">
         <v>2</v>
       </c>
-    </row>
-    <row r="117" spans="1:13">
+      <c r="N116">
+        <v>-0.8881155633500428</v>
+      </c>
+      <c r="O116">
+        <v>0.463157589730668</v>
+      </c>
+      <c r="P116">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="117" spans="1:16">
       <c r="A117" s="1" t="s">
-        <v>128</v>
+        <v>131</v>
       </c>
       <c r="B117" t="s">
-        <v>184</v>
+        <v>187</v>
       </c>
       <c r="C117">
         <v>0.31</v>
@@ -5734,13 +6787,22 @@
       <c r="M117">
         <v>3</v>
       </c>
-    </row>
-    <row r="118" spans="1:13">
+      <c r="N117">
+        <v>2.862330996024526</v>
+      </c>
+      <c r="O117">
+        <v>-1.964458199563804</v>
+      </c>
+      <c r="P117">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="118" spans="1:16">
       <c r="A118" s="1" t="s">
-        <v>129</v>
+        <v>132</v>
       </c>
       <c r="B118" t="s">
-        <v>182</v>
+        <v>185</v>
       </c>
       <c r="C118">
         <v>1.76</v>
@@ -5775,13 +6837,22 @@
       <c r="M118">
         <v>1</v>
       </c>
-    </row>
-    <row r="119" spans="1:13">
+      <c r="N118">
+        <v>-1.536900102972398</v>
+      </c>
+      <c r="O118">
+        <v>0.6376999133934023</v>
+      </c>
+      <c r="P118">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="119" spans="1:16">
       <c r="A119" s="1" t="s">
-        <v>130</v>
+        <v>133</v>
       </c>
       <c r="B119" t="s">
-        <v>184</v>
+        <v>187</v>
       </c>
       <c r="C119">
         <v>-0.1</v>
@@ -5816,13 +6887,22 @@
       <c r="M119">
         <v>3</v>
       </c>
-    </row>
-    <row r="120" spans="1:13">
+      <c r="N119">
+        <v>2.493570761786728</v>
+      </c>
+      <c r="O119">
+        <v>3.569560722293233</v>
+      </c>
+      <c r="P119">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="120" spans="1:16">
       <c r="A120" s="1" t="s">
-        <v>131</v>
+        <v>134</v>
       </c>
       <c r="B120" t="s">
-        <v>186</v>
+        <v>189</v>
       </c>
       <c r="C120">
         <v>0.51</v>
@@ -5857,13 +6937,22 @@
       <c r="M120">
         <v>3</v>
       </c>
-    </row>
-    <row r="121" spans="1:13">
+      <c r="N120">
+        <v>1.696504493501614</v>
+      </c>
+      <c r="O120">
+        <v>-0.533648638141283</v>
+      </c>
+      <c r="P120">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="121" spans="1:16">
       <c r="A121" s="1" t="s">
-        <v>132</v>
+        <v>135</v>
       </c>
       <c r="B121" t="s">
-        <v>184</v>
+        <v>187</v>
       </c>
       <c r="C121">
         <v>-0.27</v>
@@ -5898,13 +6987,22 @@
       <c r="M121">
         <v>3</v>
       </c>
-    </row>
-    <row r="122" spans="1:13">
+      <c r="N121">
+        <v>2.760765306170326</v>
+      </c>
+      <c r="O121">
+        <v>1.525832036063821</v>
+      </c>
+      <c r="P121">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="122" spans="1:16">
       <c r="A122" s="1" t="s">
-        <v>133</v>
+        <v>136</v>
       </c>
       <c r="B122" t="s">
-        <v>185</v>
+        <v>188</v>
       </c>
       <c r="C122">
         <v>1.1</v>
@@ -5939,13 +7037,22 @@
       <c r="M122">
         <v>1</v>
       </c>
-    </row>
-    <row r="123" spans="1:13">
+      <c r="N122">
+        <v>-1.872172208474265</v>
+      </c>
+      <c r="O122">
+        <v>3.485251281337218</v>
+      </c>
+      <c r="P122">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="123" spans="1:16">
       <c r="A123" s="1" t="s">
-        <v>134</v>
+        <v>137</v>
       </c>
       <c r="B123" t="s">
-        <v>184</v>
+        <v>187</v>
       </c>
       <c r="C123">
         <v>-0.66</v>
@@ -5980,13 +7087,22 @@
       <c r="M123">
         <v>3</v>
       </c>
-    </row>
-    <row r="124" spans="1:13">
+      <c r="N123">
+        <v>1.703727132477742</v>
+      </c>
+      <c r="O123">
+        <v>1.60430667835539</v>
+      </c>
+      <c r="P123">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="124" spans="1:16">
       <c r="A124" s="1" t="s">
-        <v>135</v>
+        <v>138</v>
       </c>
       <c r="B124" t="s">
-        <v>184</v>
+        <v>187</v>
       </c>
       <c r="C124">
         <v>0.86</v>
@@ -6021,13 +7137,22 @@
       <c r="M124">
         <v>3</v>
       </c>
-    </row>
-    <row r="125" spans="1:13">
+      <c r="N124">
+        <v>1.913387893753976</v>
+      </c>
+      <c r="O124">
+        <v>0.07966994167775551</v>
+      </c>
+      <c r="P124">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="125" spans="1:16">
       <c r="A125" s="1" t="s">
-        <v>136</v>
+        <v>139</v>
       </c>
       <c r="B125" t="s">
-        <v>183</v>
+        <v>186</v>
       </c>
       <c r="C125">
         <v>2.92</v>
@@ -6062,13 +7187,22 @@
       <c r="M125">
         <v>1</v>
       </c>
-    </row>
-    <row r="126" spans="1:13">
+      <c r="N125">
+        <v>-2.863006128033194</v>
+      </c>
+      <c r="O125">
+        <v>0.5170323516247394</v>
+      </c>
+      <c r="P125">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="126" spans="1:16">
       <c r="A126" s="1" t="s">
-        <v>137</v>
+        <v>140</v>
       </c>
       <c r="B126" t="s">
-        <v>183</v>
+        <v>186</v>
       </c>
       <c r="C126">
         <v>0.95</v>
@@ -6103,13 +7237,22 @@
       <c r="M126">
         <v>1</v>
       </c>
-    </row>
-    <row r="127" spans="1:13">
+      <c r="N126">
+        <v>-1.653659335348045</v>
+      </c>
+      <c r="O126">
+        <v>0.4491794567344279</v>
+      </c>
+      <c r="P126">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="127" spans="1:16">
       <c r="A127" s="1" t="s">
-        <v>138</v>
+        <v>141</v>
       </c>
       <c r="B127" t="s">
-        <v>182</v>
+        <v>185</v>
       </c>
       <c r="C127">
         <v>0.42</v>
@@ -6144,13 +7287,22 @@
       <c r="M127">
         <v>3</v>
       </c>
-    </row>
-    <row r="128" spans="1:13">
+      <c r="N127">
+        <v>1.821843801182096</v>
+      </c>
+      <c r="O127">
+        <v>1.95375460943089</v>
+      </c>
+      <c r="P127">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="128" spans="1:16">
       <c r="A128" s="1" t="s">
-        <v>139</v>
+        <v>142</v>
       </c>
       <c r="B128" t="s">
-        <v>184</v>
+        <v>187</v>
       </c>
       <c r="C128">
         <v>-0.17</v>
@@ -6185,13 +7337,22 @@
       <c r="M128">
         <v>2</v>
       </c>
-    </row>
-    <row r="129" spans="1:13">
+      <c r="N128">
+        <v>0.05407533299462614</v>
+      </c>
+      <c r="O128">
+        <v>0.4286812434382937</v>
+      </c>
+      <c r="P128">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="129" spans="1:16">
       <c r="A129" s="1" t="s">
-        <v>140</v>
+        <v>143</v>
       </c>
       <c r="B129" t="s">
-        <v>185</v>
+        <v>188</v>
       </c>
       <c r="C129">
         <v>1.26</v>
@@ -6226,13 +7387,22 @@
       <c r="M129">
         <v>2</v>
       </c>
-    </row>
-    <row r="130" spans="1:13">
+      <c r="N129">
+        <v>0.2552133375970176</v>
+      </c>
+      <c r="O129">
+        <v>-0.2157262330753536</v>
+      </c>
+      <c r="P129">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="130" spans="1:16">
       <c r="A130" s="1" t="s">
-        <v>141</v>
+        <v>144</v>
       </c>
       <c r="B130" t="s">
-        <v>182</v>
+        <v>185</v>
       </c>
       <c r="C130">
         <v>0.51</v>
@@ -6267,13 +7437,22 @@
       <c r="M130">
         <v>1</v>
       </c>
-    </row>
-    <row r="131" spans="1:13">
+      <c r="N130">
+        <v>-2.012498591175117</v>
+      </c>
+      <c r="O130">
+        <v>0.8406629109954533</v>
+      </c>
+      <c r="P130">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="131" spans="1:16">
       <c r="A131" s="1" t="s">
-        <v>142</v>
+        <v>145</v>
       </c>
       <c r="B131" t="s">
-        <v>183</v>
+        <v>186</v>
       </c>
       <c r="C131">
         <v>3.44</v>
@@ -6308,13 +7487,22 @@
       <c r="M131">
         <v>1</v>
       </c>
-    </row>
-    <row r="132" spans="1:13">
+      <c r="N131">
+        <v>-2.701216944182698</v>
+      </c>
+      <c r="O131">
+        <v>0.3342232875876797</v>
+      </c>
+      <c r="P131">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="132" spans="1:16">
       <c r="A132" s="1" t="s">
-        <v>143</v>
+        <v>146</v>
       </c>
       <c r="B132" t="s">
-        <v>185</v>
+        <v>188</v>
       </c>
       <c r="C132">
         <v>0.89</v>
@@ -6349,13 +7537,22 @@
       <c r="M132">
         <v>3</v>
       </c>
-    </row>
-    <row r="133" spans="1:13">
+      <c r="N132">
+        <v>2.100970034022984</v>
+      </c>
+      <c r="O132">
+        <v>-1.151546582605659</v>
+      </c>
+      <c r="P132">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="133" spans="1:16">
       <c r="A133" s="1" t="s">
-        <v>144</v>
+        <v>147</v>
       </c>
       <c r="B133" t="s">
-        <v>185</v>
+        <v>188</v>
       </c>
       <c r="C133">
         <v>0.12</v>
@@ -6390,13 +7587,22 @@
       <c r="M133">
         <v>3</v>
       </c>
-    </row>
-    <row r="134" spans="1:13">
+      <c r="N133">
+        <v>1.897588849777813</v>
+      </c>
+      <c r="O133">
+        <v>-1.433247605479032</v>
+      </c>
+      <c r="P133">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="134" spans="1:16">
       <c r="A134" s="1" t="s">
-        <v>145</v>
+        <v>148</v>
       </c>
       <c r="B134" t="s">
-        <v>185</v>
+        <v>188</v>
       </c>
       <c r="C134">
         <v>0.79</v>
@@ -6431,13 +7637,22 @@
       <c r="M134">
         <v>2</v>
       </c>
-    </row>
-    <row r="135" spans="1:13">
+      <c r="N134">
+        <v>1.153601787802182</v>
+      </c>
+      <c r="O134">
+        <v>-1.445402343388881</v>
+      </c>
+      <c r="P134">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="135" spans="1:16">
       <c r="A135" s="1" t="s">
-        <v>146</v>
+        <v>149</v>
       </c>
       <c r="B135" t="s">
-        <v>186</v>
+        <v>189</v>
       </c>
       <c r="C135">
         <v>0.73</v>
@@ -6472,13 +7687,22 @@
       <c r="M135">
         <v>3</v>
       </c>
-    </row>
-    <row r="136" spans="1:13">
+      <c r="N135">
+        <v>1.879818393257593</v>
+      </c>
+      <c r="O135">
+        <v>-1.352329304843894</v>
+      </c>
+      <c r="P135">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="136" spans="1:16">
       <c r="A136" s="1" t="s">
-        <v>147</v>
+        <v>150</v>
       </c>
       <c r="B136" t="s">
-        <v>183</v>
+        <v>186</v>
       </c>
       <c r="C136">
         <v>2.45</v>
@@ -6513,13 +7737,22 @@
       <c r="M136">
         <v>2</v>
       </c>
-    </row>
-    <row r="137" spans="1:13">
+      <c r="N136">
+        <v>-0.8888622477608806</v>
+      </c>
+      <c r="O136">
+        <v>-1.447645038609476</v>
+      </c>
+      <c r="P136">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="137" spans="1:16">
       <c r="A137" s="1" t="s">
-        <v>148</v>
+        <v>151</v>
       </c>
       <c r="B137" t="s">
-        <v>184</v>
+        <v>187</v>
       </c>
       <c r="C137">
         <v>-0.3</v>
@@ -6554,13 +7787,22 @@
       <c r="M137">
         <v>3</v>
       </c>
-    </row>
-    <row r="138" spans="1:13">
+      <c r="N137">
+        <v>0.4006669780944054</v>
+      </c>
+      <c r="O137">
+        <v>0.8803915203187284</v>
+      </c>
+      <c r="P137">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="138" spans="1:16">
       <c r="A138" s="1" t="s">
-        <v>149</v>
+        <v>152</v>
       </c>
       <c r="B138" t="s">
-        <v>183</v>
+        <v>186</v>
       </c>
       <c r="C138">
         <v>2.5</v>
@@ -6595,13 +7837,22 @@
       <c r="M138">
         <v>1</v>
       </c>
-    </row>
-    <row r="139" spans="1:13">
+      <c r="N138">
+        <v>-2.147612694982828</v>
+      </c>
+      <c r="O138">
+        <v>-0.258630409988477</v>
+      </c>
+      <c r="P138">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="139" spans="1:16">
       <c r="A139" s="1" t="s">
-        <v>150</v>
+        <v>153</v>
       </c>
       <c r="B139" t="s">
-        <v>184</v>
+        <v>187</v>
       </c>
       <c r="C139">
         <v>0.09</v>
@@ -6636,13 +7887,22 @@
       <c r="M139">
         <v>3</v>
       </c>
-    </row>
-    <row r="140" spans="1:13">
+      <c r="N139">
+        <v>1.72992249125999</v>
+      </c>
+      <c r="O139">
+        <v>-0.001588823098311626</v>
+      </c>
+      <c r="P139">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="140" spans="1:16">
       <c r="A140" s="1" t="s">
-        <v>151</v>
+        <v>154</v>
       </c>
       <c r="B140" t="s">
-        <v>184</v>
+        <v>187</v>
       </c>
       <c r="C140">
         <v>0.32</v>
@@ -6677,13 +7937,22 @@
       <c r="M140">
         <v>3</v>
       </c>
-    </row>
-    <row r="141" spans="1:13">
+      <c r="N140">
+        <v>1.784085117189915</v>
+      </c>
+      <c r="O140">
+        <v>0.2870982013102065</v>
+      </c>
+      <c r="P140">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="141" spans="1:16">
       <c r="A141" s="1" t="s">
-        <v>152</v>
+        <v>155</v>
       </c>
       <c r="B141" t="s">
-        <v>183</v>
+        <v>186</v>
       </c>
       <c r="C141">
         <v>2.32</v>
@@ -6718,13 +7987,22 @@
       <c r="M141">
         <v>1</v>
       </c>
-    </row>
-    <row r="142" spans="1:13">
+      <c r="N141">
+        <v>-2.897618485890634</v>
+      </c>
+      <c r="O141">
+        <v>1.108557428000389</v>
+      </c>
+      <c r="P141">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="142" spans="1:16">
       <c r="A142" s="1" t="s">
-        <v>153</v>
+        <v>156</v>
       </c>
       <c r="B142" t="s">
-        <v>182</v>
+        <v>185</v>
       </c>
       <c r="C142">
         <v>0.65</v>
@@ -6759,13 +8037,22 @@
       <c r="M142">
         <v>1</v>
       </c>
-    </row>
-    <row r="143" spans="1:13">
+      <c r="N142">
+        <v>-1.715484866620011</v>
+      </c>
+      <c r="O142">
+        <v>1.153903474014053</v>
+      </c>
+      <c r="P142">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="143" spans="1:16">
       <c r="A143" s="1" t="s">
-        <v>154</v>
+        <v>157</v>
       </c>
       <c r="B143" t="s">
-        <v>184</v>
+        <v>187</v>
       </c>
       <c r="C143">
         <v>1.22</v>
@@ -6800,13 +8087,22 @@
       <c r="M143">
         <v>3</v>
       </c>
-    </row>
-    <row r="144" spans="1:13">
+      <c r="N143">
+        <v>2.842506832321542</v>
+      </c>
+      <c r="O143">
+        <v>0.2207747001046948</v>
+      </c>
+      <c r="P143">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="144" spans="1:16">
       <c r="A144" s="1" t="s">
-        <v>155</v>
+        <v>158</v>
       </c>
       <c r="B144" t="s">
-        <v>185</v>
+        <v>188</v>
       </c>
       <c r="C144">
         <v>1.16</v>
@@ -6841,13 +8137,22 @@
       <c r="M144">
         <v>2</v>
       </c>
-    </row>
-    <row r="145" spans="1:13">
+      <c r="N144">
+        <v>0.2670560630335576</v>
+      </c>
+      <c r="O144">
+        <v>-1.02905946830546</v>
+      </c>
+      <c r="P144">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="145" spans="1:16">
       <c r="A145" s="1" t="s">
-        <v>156</v>
+        <v>159</v>
       </c>
       <c r="B145" t="s">
-        <v>184</v>
+        <v>187</v>
       </c>
       <c r="C145">
         <v>0.8100000000000001</v>
@@ -6882,13 +8187,22 @@
       <c r="M145">
         <v>3</v>
       </c>
-    </row>
-    <row r="146" spans="1:13">
+      <c r="N145">
+        <v>2.763114756521933</v>
+      </c>
+      <c r="O145">
+        <v>0.6332484005389376</v>
+      </c>
+      <c r="P145">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="146" spans="1:16">
       <c r="A146" s="1" t="s">
-        <v>157</v>
+        <v>160</v>
       </c>
       <c r="B146" t="s">
-        <v>183</v>
+        <v>186</v>
       </c>
       <c r="C146">
         <v>3.19</v>
@@ -6923,13 +8237,22 @@
       <c r="M146">
         <v>1</v>
       </c>
-    </row>
-    <row r="147" spans="1:13">
+      <c r="N146">
+        <v>-2.378852637146996</v>
+      </c>
+      <c r="O146">
+        <v>0.4298357572845043</v>
+      </c>
+      <c r="P146">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="147" spans="1:16">
       <c r="A147" s="1" t="s">
-        <v>158</v>
+        <v>161</v>
       </c>
       <c r="B147" t="s">
-        <v>182</v>
+        <v>185</v>
       </c>
       <c r="C147">
         <v>2.57</v>
@@ -6964,13 +8287,22 @@
       <c r="M147">
         <v>2</v>
       </c>
-    </row>
-    <row r="148" spans="1:13">
+      <c r="N147">
+        <v>-1.31552977367585</v>
+      </c>
+      <c r="O147">
+        <v>-0.9177270578824227</v>
+      </c>
+      <c r="P147">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="148" spans="1:16">
       <c r="A148" s="1" t="s">
-        <v>159</v>
+        <v>162</v>
       </c>
       <c r="B148" t="s">
-        <v>183</v>
+        <v>186</v>
       </c>
       <c r="C148">
         <v>3.88</v>
@@ -7005,13 +8337,22 @@
       <c r="M148">
         <v>1</v>
       </c>
-    </row>
-    <row r="149" spans="1:13">
+      <c r="N148">
+        <v>-2.09331186682009</v>
+      </c>
+      <c r="O148">
+        <v>-0.06816611263679713</v>
+      </c>
+      <c r="P148">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="149" spans="1:16">
       <c r="A149" s="1" t="s">
-        <v>160</v>
+        <v>163</v>
       </c>
       <c r="B149" t="s">
-        <v>184</v>
+        <v>187</v>
       </c>
       <c r="C149">
         <v>0.27</v>
@@ -7046,13 +8387,22 @@
       <c r="M149">
         <v>3</v>
       </c>
-    </row>
-    <row r="150" spans="1:13">
+      <c r="N149">
+        <v>2.021308092662168</v>
+      </c>
+      <c r="O149">
+        <v>0.2072484993458034</v>
+      </c>
+      <c r="P149">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="150" spans="1:16">
       <c r="A150" s="1" t="s">
-        <v>161</v>
+        <v>164</v>
       </c>
       <c r="B150" t="s">
-        <v>182</v>
+        <v>185</v>
       </c>
       <c r="C150">
         <v>0.46</v>
@@ -7087,13 +8437,22 @@
       <c r="M150">
         <v>1</v>
       </c>
-    </row>
-    <row r="151" spans="1:13">
+      <c r="N150">
+        <v>-0.9550813321237719</v>
+      </c>
+      <c r="O150">
+        <v>1.188064451289703</v>
+      </c>
+      <c r="P150">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="151" spans="1:16">
       <c r="A151" s="1" t="s">
-        <v>162</v>
+        <v>165</v>
       </c>
       <c r="B151" t="s">
-        <v>182</v>
+        <v>185</v>
       </c>
       <c r="C151">
         <v>2</v>
@@ -7128,13 +8487,22 @@
       <c r="M151">
         <v>2</v>
       </c>
-    </row>
-    <row r="152" spans="1:13">
+      <c r="N151">
+        <v>-1.021051831365606</v>
+      </c>
+      <c r="O151">
+        <v>-2.452410813063677</v>
+      </c>
+      <c r="P151">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="152" spans="1:16">
       <c r="A152" s="1" t="s">
-        <v>163</v>
+        <v>166</v>
       </c>
       <c r="B152" t="s">
-        <v>183</v>
+        <v>186</v>
       </c>
       <c r="C152">
         <v>3</v>
@@ -7169,13 +8537,22 @@
       <c r="M152">
         <v>2</v>
       </c>
-    </row>
-    <row r="153" spans="1:13">
+      <c r="N152">
+        <v>-2.024037750979055</v>
+      </c>
+      <c r="O152">
+        <v>-0.993275688759349</v>
+      </c>
+      <c r="P152">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="153" spans="1:16">
       <c r="A153" s="1" t="s">
-        <v>164</v>
+        <v>167</v>
       </c>
       <c r="B153" t="s">
-        <v>185</v>
+        <v>188</v>
       </c>
       <c r="C153">
         <v>0.58</v>
@@ -7210,13 +8587,22 @@
       <c r="M153">
         <v>3</v>
       </c>
-    </row>
-    <row r="154" spans="1:13">
+      <c r="N153">
+        <v>1.112713194210416</v>
+      </c>
+      <c r="O153">
+        <v>-0.1410020455683317</v>
+      </c>
+      <c r="P153">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="154" spans="1:16">
       <c r="A154" s="1" t="s">
-        <v>165</v>
+        <v>168</v>
       </c>
       <c r="B154" t="s">
-        <v>183</v>
+        <v>186</v>
       </c>
       <c r="C154">
         <v>1.1</v>
@@ -7251,13 +8637,22 @@
       <c r="M154">
         <v>2</v>
       </c>
-    </row>
-    <row r="155" spans="1:13">
+      <c r="N154">
+        <v>-0.8840009128278439</v>
+      </c>
+      <c r="O154">
+        <v>0.3317488795957917</v>
+      </c>
+      <c r="P154">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="155" spans="1:16">
       <c r="A155" s="1" t="s">
-        <v>166</v>
+        <v>169</v>
       </c>
       <c r="B155" t="s">
-        <v>182</v>
+        <v>185</v>
       </c>
       <c r="C155">
         <v>1.82</v>
@@ -7292,13 +8687,22 @@
       <c r="M155">
         <v>1</v>
       </c>
-    </row>
-    <row r="156" spans="1:13">
+      <c r="N155">
+        <v>-0.5673870312280181</v>
+      </c>
+      <c r="O155">
+        <v>0.5793411718427858</v>
+      </c>
+      <c r="P155">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="156" spans="1:16">
       <c r="A156" s="1" t="s">
-        <v>167</v>
+        <v>170</v>
       </c>
       <c r="B156" t="s">
-        <v>182</v>
+        <v>185</v>
       </c>
       <c r="C156">
         <v>1.66</v>
@@ -7333,13 +8737,22 @@
       <c r="M156">
         <v>2</v>
       </c>
-    </row>
-    <row r="157" spans="1:13">
+      <c r="N156">
+        <v>-0.2273244007129689</v>
+      </c>
+      <c r="O156">
+        <v>1.398835882350266</v>
+      </c>
+      <c r="P156">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="157" spans="1:16">
       <c r="A157" s="1" t="s">
-        <v>168</v>
+        <v>171</v>
       </c>
       <c r="B157" t="s">
-        <v>184</v>
+        <v>187</v>
       </c>
       <c r="C157">
         <v>-0.41</v>
@@ -7374,13 +8787,22 @@
       <c r="M157">
         <v>2</v>
       </c>
-    </row>
-    <row r="158" spans="1:13">
+      <c r="N157">
+        <v>0.1326324985279513</v>
+      </c>
+      <c r="O157">
+        <v>1.261014209304824</v>
+      </c>
+      <c r="P157">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="158" spans="1:16">
       <c r="A158" s="1" t="s">
-        <v>169</v>
+        <v>172</v>
       </c>
       <c r="B158" t="s">
-        <v>185</v>
+        <v>188</v>
       </c>
       <c r="C158">
         <v>0.31</v>
@@ -7415,13 +8837,22 @@
       <c r="M158">
         <v>3</v>
       </c>
-    </row>
-    <row r="159" spans="1:13">
+      <c r="N158">
+        <v>1.046608077533504</v>
+      </c>
+      <c r="O158">
+        <v>0.6997860794083995</v>
+      </c>
+      <c r="P158">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="159" spans="1:16">
       <c r="A159" s="1" t="s">
-        <v>170</v>
+        <v>173</v>
       </c>
       <c r="B159" t="s">
-        <v>186</v>
+        <v>189</v>
       </c>
       <c r="C159">
         <v>3.01</v>
@@ -7456,13 +8887,22 @@
       <c r="M159">
         <v>2</v>
       </c>
-    </row>
-    <row r="160" spans="1:13">
+      <c r="N159">
+        <v>-0.04238633276435765</v>
+      </c>
+      <c r="O159">
+        <v>-1.876649537546447</v>
+      </c>
+      <c r="P159">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="160" spans="1:16">
       <c r="A160" s="1" t="s">
-        <v>171</v>
+        <v>174</v>
       </c>
       <c r="B160" t="s">
-        <v>185</v>
+        <v>188</v>
       </c>
       <c r="C160">
         <v>0.79</v>
@@ -7497,13 +8937,22 @@
       <c r="M160">
         <v>2</v>
       </c>
-    </row>
-    <row r="161" spans="1:13">
+      <c r="N160">
+        <v>-1.153904848852118</v>
+      </c>
+      <c r="O160">
+        <v>0.8425528650636078</v>
+      </c>
+      <c r="P160">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="161" spans="1:16">
       <c r="A161" s="1" t="s">
-        <v>172</v>
+        <v>175</v>
       </c>
       <c r="B161" t="s">
-        <v>182</v>
+        <v>185</v>
       </c>
       <c r="C161">
         <v>1.07</v>
@@ -7538,13 +8987,22 @@
       <c r="M161">
         <v>2</v>
       </c>
-    </row>
-    <row r="162" spans="1:13">
+      <c r="N161">
+        <v>-0.6525445255282016</v>
+      </c>
+      <c r="O161">
+        <v>0.5728478913787673</v>
+      </c>
+      <c r="P161">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="162" spans="1:16">
       <c r="A162" s="1" t="s">
-        <v>173</v>
+        <v>176</v>
       </c>
       <c r="B162" t="s">
-        <v>182</v>
+        <v>185</v>
       </c>
       <c r="C162">
         <v>3.08</v>
@@ -7579,13 +9037,22 @@
       <c r="M162">
         <v>1</v>
       </c>
-    </row>
-    <row r="163" spans="1:13">
+      <c r="N162">
+        <v>-3.18972620425904</v>
+      </c>
+      <c r="O162">
+        <v>-0.3956963572848236</v>
+      </c>
+      <c r="P162">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="163" spans="1:16">
       <c r="A163" s="1" t="s">
-        <v>174</v>
+        <v>177</v>
       </c>
       <c r="B163" t="s">
-        <v>183</v>
+        <v>186</v>
       </c>
       <c r="C163">
         <v>3.48</v>
@@ -7620,13 +9087,22 @@
       <c r="M163">
         <v>1</v>
       </c>
-    </row>
-    <row r="164" spans="1:13">
+      <c r="N163">
+        <v>-1.990088673967854</v>
+      </c>
+      <c r="O163">
+        <v>-0.1710949192806485</v>
+      </c>
+      <c r="P163">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="164" spans="1:16">
       <c r="A164" s="1" t="s">
-        <v>175</v>
+        <v>178</v>
       </c>
       <c r="B164" t="s">
-        <v>183</v>
+        <v>186</v>
       </c>
       <c r="C164">
         <v>1.62</v>
@@ -7661,13 +9137,22 @@
       <c r="M164">
         <v>1</v>
       </c>
-    </row>
-    <row r="165" spans="1:13">
+      <c r="N164">
+        <v>-2.095131561903889</v>
+      </c>
+      <c r="O164">
+        <v>0.7238160788862812</v>
+      </c>
+      <c r="P164">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="165" spans="1:16">
       <c r="A165" s="1" t="s">
-        <v>176</v>
+        <v>179</v>
       </c>
       <c r="B165" t="s">
-        <v>183</v>
+        <v>186</v>
       </c>
       <c r="C165">
         <v>2.33</v>
@@ -7702,13 +9187,22 @@
       <c r="M165">
         <v>2</v>
       </c>
-    </row>
-    <row r="166" spans="1:13">
+      <c r="N165">
+        <v>-1.757518204989799</v>
+      </c>
+      <c r="O165">
+        <v>-0.3702081374257244</v>
+      </c>
+      <c r="P165">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="166" spans="1:16">
       <c r="A166" s="1" t="s">
-        <v>177</v>
+        <v>180</v>
       </c>
       <c r="B166" t="s">
-        <v>182</v>
+        <v>185</v>
       </c>
       <c r="C166">
         <v>5.38</v>
@@ -7743,13 +9237,22 @@
       <c r="M166">
         <v>2</v>
       </c>
-    </row>
-    <row r="167" spans="1:13">
+      <c r="N166">
+        <v>0.7049558865422446</v>
+      </c>
+      <c r="O166">
+        <v>-3.085007322401323</v>
+      </c>
+      <c r="P166">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="167" spans="1:16">
       <c r="A167" s="1" t="s">
-        <v>178</v>
+        <v>181</v>
       </c>
       <c r="B167" t="s">
-        <v>185</v>
+        <v>188</v>
       </c>
       <c r="C167">
         <v>1.74</v>
@@ -7784,13 +9287,22 @@
       <c r="M167">
         <v>1</v>
       </c>
-    </row>
-    <row r="168" spans="1:13">
+      <c r="N167">
+        <v>-0.8773260658399902</v>
+      </c>
+      <c r="O167">
+        <v>0.8701663938869357</v>
+      </c>
+      <c r="P167">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="168" spans="1:16">
       <c r="A168" s="1" t="s">
-        <v>179</v>
+        <v>182</v>
       </c>
       <c r="B168" t="s">
-        <v>185</v>
+        <v>188</v>
       </c>
       <c r="C168">
         <v>0.8100000000000001</v>
@@ -7825,13 +9337,22 @@
       <c r="M168">
         <v>3</v>
       </c>
-    </row>
-    <row r="169" spans="1:13">
+      <c r="N168">
+        <v>3.044527383230702</v>
+      </c>
+      <c r="O168">
+        <v>1.45380750321847</v>
+      </c>
+      <c r="P168">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="169" spans="1:16">
       <c r="A169" s="1" t="s">
-        <v>180</v>
+        <v>183</v>
       </c>
       <c r="B169" t="s">
-        <v>183</v>
+        <v>186</v>
       </c>
       <c r="C169">
         <v>3.19</v>
@@ -7866,13 +9387,22 @@
       <c r="M169">
         <v>1</v>
       </c>
-    </row>
-    <row r="170" spans="1:13">
+      <c r="N169">
+        <v>-3.942463504383146</v>
+      </c>
+      <c r="O169">
+        <v>0.9138175500458366</v>
+      </c>
+      <c r="P169">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="170" spans="1:16">
       <c r="A170" s="1" t="s">
-        <v>181</v>
+        <v>184</v>
       </c>
       <c r="B170" t="s">
-        <v>186</v>
+        <v>189</v>
       </c>
       <c r="C170">
         <v>2.92</v>
@@ -7906,6 +9436,15 @@
       </c>
       <c r="M170">
         <v>2</v>
+      </c>
+      <c r="N170">
+        <v>-0.8318012892608124</v>
+      </c>
+      <c r="O170">
+        <v>-2.580421345317528</v>
+      </c>
+      <c r="P170">
+        <v>4</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Correction post-soutenance : 5 clusters kmeans
</commit_message>
<xml_diff>
--- a/DonnéesFinales.xlsx
+++ b/DonnéesFinales.xlsx
@@ -1085,7 +1085,7 @@
         <v>3</v>
       </c>
       <c r="M3">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="N3">
         <v>-0.2430651747344462</v>
@@ -1135,7 +1135,7 @@
         <v>3</v>
       </c>
       <c r="M4">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="N4">
         <v>1.23711174845644</v>
@@ -1235,7 +1235,7 @@
         <v>1</v>
       </c>
       <c r="M6">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="N6">
         <v>2.374576960373252</v>
@@ -1285,7 +1285,7 @@
         <v>4</v>
       </c>
       <c r="M7">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="N7">
         <v>-1.589117576938125</v>
@@ -1335,7 +1335,7 @@
         <v>3</v>
       </c>
       <c r="M8">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="N8">
         <v>2.486553824461864</v>
@@ -1385,7 +1385,7 @@
         <v>3</v>
       </c>
       <c r="M9">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="N9">
         <v>-0.1219779925040396</v>
@@ -1435,7 +1435,7 @@
         <v>3</v>
       </c>
       <c r="M10">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="N10">
         <v>1.073744356574197</v>
@@ -1485,7 +1485,7 @@
         <v>3</v>
       </c>
       <c r="M11">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="N11">
         <v>0.5177970501459672</v>
@@ -1535,7 +1535,7 @@
         <v>2</v>
       </c>
       <c r="M12">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="N12">
         <v>2.826622072555177</v>
@@ -1585,7 +1585,7 @@
         <v>1</v>
       </c>
       <c r="M13">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="N13">
         <v>2.698326469749897</v>
@@ -1635,7 +1635,7 @@
         <v>5</v>
       </c>
       <c r="M14">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="N14">
         <v>-0.6722339071837684</v>
@@ -1685,7 +1685,7 @@
         <v>3</v>
       </c>
       <c r="M15">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="N15">
         <v>2.956253395604683</v>
@@ -1785,7 +1785,7 @@
         <v>3</v>
       </c>
       <c r="M17">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="N17">
         <v>1.490072988841497</v>
@@ -1835,7 +1835,7 @@
         <v>1</v>
       </c>
       <c r="M18">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="N18">
         <v>2.549916646807758</v>
@@ -1885,7 +1885,7 @@
         <v>3</v>
       </c>
       <c r="M19">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="N19">
         <v>-0.5601540678275257</v>
@@ -1985,7 +1985,7 @@
         <v>3</v>
       </c>
       <c r="M21">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="N21">
         <v>0.04767303901981641</v>
@@ -2035,7 +2035,7 @@
         <v>4</v>
       </c>
       <c r="M22">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="N22">
         <v>0.1194282815915174</v>
@@ -2085,7 +2085,7 @@
         <v>3</v>
       </c>
       <c r="M23">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="N23">
         <v>0.8634100196819752</v>
@@ -2135,7 +2135,7 @@
         <v>3</v>
       </c>
       <c r="M24">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="N24">
         <v>1.119840707834355</v>
@@ -2235,7 +2235,7 @@
         <v>2</v>
       </c>
       <c r="M26">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="N26">
         <v>1.171974536052488</v>
@@ -2285,7 +2285,7 @@
         <v>4</v>
       </c>
       <c r="M27">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="N27">
         <v>-1.388431971708215</v>
@@ -2335,7 +2335,7 @@
         <v>4</v>
       </c>
       <c r="M28">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="N28">
         <v>0.1745598253830776</v>
@@ -2485,7 +2485,7 @@
         <v>3</v>
       </c>
       <c r="M31">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="N31">
         <v>2.085703052428027</v>
@@ -2535,7 +2535,7 @@
         <v>2</v>
       </c>
       <c r="M32">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="N32">
         <v>1.403200280242539</v>
@@ -2585,7 +2585,7 @@
         <v>1</v>
       </c>
       <c r="M33">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="N33">
         <v>4.582873653459127</v>
@@ -2635,7 +2635,7 @@
         <v>1</v>
       </c>
       <c r="M34">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="N34">
         <v>4.187575663247816</v>
@@ -2685,7 +2685,7 @@
         <v>3</v>
       </c>
       <c r="M35">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="N35">
         <v>1.728456868555041</v>
@@ -2735,7 +2735,7 @@
         <v>5</v>
       </c>
       <c r="M36">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="N36">
         <v>-0.821059994714319</v>
@@ -2785,7 +2785,7 @@
         <v>3</v>
       </c>
       <c r="M37">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="N37">
         <v>1.231623805191735</v>
@@ -2835,7 +2835,7 @@
         <v>5</v>
       </c>
       <c r="M38">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="N38">
         <v>-0.8331354868731673</v>
@@ -2885,7 +2885,7 @@
         <v>4</v>
       </c>
       <c r="M39">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="N39">
         <v>-0.6504530601987876</v>
@@ -2935,7 +2935,7 @@
         <v>3</v>
       </c>
       <c r="M40">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="N40">
         <v>0.966752995214375</v>
@@ -2985,7 +2985,7 @@
         <v>3</v>
       </c>
       <c r="M41">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="N41">
         <v>1.760074424316073</v>
@@ -3035,7 +3035,7 @@
         <v>3</v>
       </c>
       <c r="M42">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="N42">
         <v>0.3858076828040779</v>
@@ -3135,7 +3135,7 @@
         <v>1</v>
       </c>
       <c r="M44">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="N44">
         <v>3.251810880785572</v>
@@ -3185,7 +3185,7 @@
         <v>4</v>
       </c>
       <c r="M45">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="N45">
         <v>-1.35325525969493</v>
@@ -3235,7 +3235,7 @@
         <v>3</v>
       </c>
       <c r="M46">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="N46">
         <v>1.617639366730089</v>
@@ -3285,7 +3285,7 @@
         <v>3</v>
       </c>
       <c r="M47">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="N47">
         <v>-0.3381301914238785</v>
@@ -3335,7 +3335,7 @@
         <v>3</v>
       </c>
       <c r="M48">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="N48">
         <v>1.560786417013898</v>
@@ -3385,7 +3385,7 @@
         <v>3</v>
       </c>
       <c r="M49">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="N49">
         <v>1.844958915753119</v>
@@ -3435,7 +3435,7 @@
         <v>5</v>
       </c>
       <c r="M50">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="N50">
         <v>-1.054220515687911</v>
@@ -3485,7 +3485,7 @@
         <v>3</v>
       </c>
       <c r="M51">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="N51">
         <v>0.1622517174532253</v>
@@ -3535,7 +3535,7 @@
         <v>1</v>
       </c>
       <c r="M52">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="N52">
         <v>2.867098374644427</v>
@@ -3585,7 +3585,7 @@
         <v>2</v>
       </c>
       <c r="M53">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="N53">
         <v>2.692564839841622</v>
@@ -3635,7 +3635,7 @@
         <v>3</v>
       </c>
       <c r="M54">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="N54">
         <v>0.6595027712872306</v>
@@ -3685,7 +3685,7 @@
         <v>4</v>
       </c>
       <c r="M55">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="N55">
         <v>0.1679313319953225</v>
@@ -3735,7 +3735,7 @@
         <v>4</v>
       </c>
       <c r="M56">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="N56">
         <v>-1.067700594946762</v>
@@ -3785,7 +3785,7 @@
         <v>4</v>
       </c>
       <c r="M57">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="N57">
         <v>-1.415824205721199</v>
@@ -3835,7 +3835,7 @@
         <v>3</v>
       </c>
       <c r="M58">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="N58">
         <v>0.6665222289851778</v>
@@ -3885,7 +3885,7 @@
         <v>2</v>
       </c>
       <c r="M59">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="N59">
         <v>1.949585554785702</v>
@@ -3935,7 +3935,7 @@
         <v>3</v>
       </c>
       <c r="M60">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="N60">
         <v>-1.527730856160604</v>
@@ -4035,7 +4035,7 @@
         <v>4</v>
       </c>
       <c r="M62">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="N62">
         <v>-2.046093232551849</v>
@@ -4085,7 +4085,7 @@
         <v>3</v>
       </c>
       <c r="M63">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="N63">
         <v>-0.06661315170382999</v>
@@ -4135,7 +4135,7 @@
         <v>3</v>
       </c>
       <c r="M64">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="N64">
         <v>-0.09489274267863565</v>
@@ -4185,7 +4185,7 @@
         <v>4</v>
       </c>
       <c r="M65">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="N65">
         <v>-1.663095372376173</v>
@@ -4235,7 +4235,7 @@
         <v>3</v>
       </c>
       <c r="M66">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="N66">
         <v>-1.137290023422126</v>
@@ -4285,7 +4285,7 @@
         <v>2</v>
       </c>
       <c r="M67">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="N67">
         <v>1.332337469712288</v>
@@ -4435,7 +4435,7 @@
         <v>3</v>
       </c>
       <c r="M70">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="N70">
         <v>-1.405257666849225</v>
@@ -4485,7 +4485,7 @@
         <v>5</v>
       </c>
       <c r="M71">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="N71">
         <v>-2.314101276316944</v>
@@ -4535,7 +4535,7 @@
         <v>1</v>
       </c>
       <c r="M72">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="N72">
         <v>3.233010929132727</v>
@@ -4585,7 +4585,7 @@
         <v>1</v>
       </c>
       <c r="M73">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="N73">
         <v>3.809891268781054</v>
@@ -4635,7 +4635,7 @@
         <v>3</v>
       </c>
       <c r="M74">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="N74">
         <v>0.8979008120174493</v>
@@ -4685,7 +4685,7 @@
         <v>2</v>
       </c>
       <c r="M75">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="N75">
         <v>1.676589959742453</v>
@@ -4735,7 +4735,7 @@
         <v>3</v>
       </c>
       <c r="M76">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="N76">
         <v>0.4942683749356915</v>
@@ -4785,7 +4785,7 @@
         <v>4</v>
       </c>
       <c r="M77">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="N77">
         <v>-1.441317317900737</v>
@@ -4835,7 +4835,7 @@
         <v>3</v>
       </c>
       <c r="M78">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="N78">
         <v>1.127787243384577</v>
@@ -4935,7 +4935,7 @@
         <v>4</v>
       </c>
       <c r="M80">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="N80">
         <v>-0.8444323358045106</v>
@@ -4985,7 +4985,7 @@
         <v>4</v>
       </c>
       <c r="M81">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="N81">
         <v>0.4682589498859397</v>
@@ -5035,7 +5035,7 @@
         <v>4</v>
       </c>
       <c r="M82">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="N82">
         <v>0.6315912275171686</v>
@@ -5085,7 +5085,7 @@
         <v>4</v>
       </c>
       <c r="M83">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="N83">
         <v>-0.7321107015493511</v>
@@ -5135,7 +5135,7 @@
         <v>3</v>
       </c>
       <c r="M84">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="N84">
         <v>2.191302444158779</v>
@@ -5185,7 +5185,7 @@
         <v>5</v>
       </c>
       <c r="M85">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="N85">
         <v>-1.975405218846225</v>
@@ -5235,7 +5235,7 @@
         <v>4</v>
       </c>
       <c r="M86">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="N86">
         <v>-1.631348833586898</v>
@@ -5285,7 +5285,7 @@
         <v>3</v>
       </c>
       <c r="M87">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="N87">
         <v>2.703898311725352</v>
@@ -5335,7 +5335,7 @@
         <v>1</v>
       </c>
       <c r="M88">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="N88">
         <v>3.907550465060897</v>
@@ -5385,7 +5385,7 @@
         <v>3</v>
       </c>
       <c r="M89">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="N89">
         <v>0.3281202388129153</v>
@@ -5485,7 +5485,7 @@
         <v>2</v>
       </c>
       <c r="M91">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="N91">
         <v>0.8866808434193805</v>
@@ -5585,7 +5585,7 @@
         <v>4</v>
       </c>
       <c r="M93">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="N93">
         <v>-0.5796046346578471</v>
@@ -5685,7 +5685,7 @@
         <v>3</v>
       </c>
       <c r="M95">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="N95">
         <v>2.378466844517986</v>
@@ -5735,7 +5735,7 @@
         <v>3</v>
       </c>
       <c r="M96">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="N96">
         <v>-0.9417386103220493</v>
@@ -5785,7 +5785,7 @@
         <v>3</v>
       </c>
       <c r="M97">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="N97">
         <v>0.9476125331007231</v>
@@ -5835,7 +5835,7 @@
         <v>4</v>
       </c>
       <c r="M98">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="N98">
         <v>-1.136704804996464</v>
@@ -5885,7 +5885,7 @@
         <v>5</v>
       </c>
       <c r="M99">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="N99">
         <v>-0.3180309088225146</v>
@@ -5935,7 +5935,7 @@
         <v>3</v>
       </c>
       <c r="M100">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="N100">
         <v>1.845190267584877</v>
@@ -5985,7 +5985,7 @@
         <v>3</v>
       </c>
       <c r="M101">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="N101">
         <v>1.827381922225326</v>
@@ -6085,7 +6085,7 @@
         <v>5</v>
       </c>
       <c r="M103">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="N103">
         <v>-0.5928194637564239</v>
@@ -6135,7 +6135,7 @@
         <v>4</v>
       </c>
       <c r="M104">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="N104">
         <v>-0.06449091935328302</v>
@@ -6185,7 +6185,7 @@
         <v>3</v>
       </c>
       <c r="M105">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="N105">
         <v>-0.9271542863218917</v>
@@ -6335,7 +6335,7 @@
         <v>1</v>
       </c>
       <c r="M108">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="N108">
         <v>2.648142771181356</v>
@@ -6385,7 +6385,7 @@
         <v>3</v>
       </c>
       <c r="M109">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="N109">
         <v>1.632198370419451</v>
@@ -6435,7 +6435,7 @@
         <v>3</v>
       </c>
       <c r="M110">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="N110">
         <v>2.154962747402586</v>
@@ -6535,7 +6535,7 @@
         <v>4</v>
       </c>
       <c r="M112">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="N112">
         <v>0.1103633206185996</v>
@@ -6685,7 +6685,7 @@
         <v>3</v>
       </c>
       <c r="M115">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="N115">
         <v>0.7926376806236393</v>
@@ -6735,7 +6735,7 @@
         <v>5</v>
       </c>
       <c r="M116">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="N116">
         <v>-0.8881155633500428</v>
@@ -6785,7 +6785,7 @@
         <v>1</v>
       </c>
       <c r="M117">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="N117">
         <v>2.862330996024526</v>
@@ -6885,7 +6885,7 @@
         <v>2</v>
       </c>
       <c r="M119">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="N119">
         <v>2.493570761786728</v>
@@ -6935,7 +6935,7 @@
         <v>3</v>
       </c>
       <c r="M120">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="N120">
         <v>1.696504493501614</v>
@@ -6985,7 +6985,7 @@
         <v>2</v>
       </c>
       <c r="M121">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="N121">
         <v>2.760765306170326</v>
@@ -7085,7 +7085,7 @@
         <v>2</v>
       </c>
       <c r="M123">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="N123">
         <v>1.703727132477742</v>
@@ -7135,7 +7135,7 @@
         <v>3</v>
       </c>
       <c r="M124">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="N124">
         <v>1.913387893753976</v>
@@ -7285,7 +7285,7 @@
         <v>2</v>
       </c>
       <c r="M127">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="N127">
         <v>1.821843801182096</v>
@@ -7335,7 +7335,7 @@
         <v>3</v>
       </c>
       <c r="M128">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="N128">
         <v>0.05407533299462614</v>
@@ -7385,7 +7385,7 @@
         <v>3</v>
       </c>
       <c r="M129">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="N129">
         <v>0.2552133375970176</v>
@@ -7535,7 +7535,7 @@
         <v>3</v>
       </c>
       <c r="M132">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="N132">
         <v>2.100970034022984</v>
@@ -7585,7 +7585,7 @@
         <v>3</v>
       </c>
       <c r="M133">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="N133">
         <v>1.897588849777813</v>
@@ -7635,7 +7635,7 @@
         <v>3</v>
       </c>
       <c r="M134">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="N134">
         <v>1.153601787802182</v>
@@ -7685,7 +7685,7 @@
         <v>3</v>
       </c>
       <c r="M135">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="N135">
         <v>1.879818393257593</v>
@@ -7735,7 +7735,7 @@
         <v>4</v>
       </c>
       <c r="M136">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="N136">
         <v>-0.8888622477608806</v>
@@ -7785,7 +7785,7 @@
         <v>3</v>
       </c>
       <c r="M137">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="N137">
         <v>0.4006669780944054</v>
@@ -7885,7 +7885,7 @@
         <v>3</v>
       </c>
       <c r="M139">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="N139">
         <v>1.72992249125999</v>
@@ -7935,7 +7935,7 @@
         <v>3</v>
       </c>
       <c r="M140">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="N140">
         <v>1.784085117189915</v>
@@ -8085,7 +8085,7 @@
         <v>1</v>
       </c>
       <c r="M143">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="N143">
         <v>2.842506832321542</v>
@@ -8135,7 +8135,7 @@
         <v>3</v>
       </c>
       <c r="M144">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="N144">
         <v>0.2670560630335576</v>
@@ -8185,7 +8185,7 @@
         <v>1</v>
       </c>
       <c r="M145">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="N145">
         <v>2.763114756521933</v>
@@ -8285,7 +8285,7 @@
         <v>4</v>
       </c>
       <c r="M147">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="N147">
         <v>-1.31552977367585</v>
@@ -8385,7 +8385,7 @@
         <v>3</v>
       </c>
       <c r="M149">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="N149">
         <v>2.021308092662168</v>
@@ -8435,7 +8435,7 @@
         <v>5</v>
       </c>
       <c r="M150">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="N150">
         <v>-0.9550813321237719</v>
@@ -8485,7 +8485,7 @@
         <v>4</v>
       </c>
       <c r="M151">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="N151">
         <v>-1.021051831365606</v>
@@ -8535,7 +8535,7 @@
         <v>4</v>
       </c>
       <c r="M152">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="N152">
         <v>-2.024037750979055</v>
@@ -8585,7 +8585,7 @@
         <v>3</v>
       </c>
       <c r="M153">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="N153">
         <v>1.112713194210416</v>
@@ -8635,7 +8635,7 @@
         <v>3</v>
       </c>
       <c r="M154">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="N154">
         <v>-0.8840009128278439</v>
@@ -8785,7 +8785,7 @@
         <v>3</v>
       </c>
       <c r="M157">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="N157">
         <v>0.1326324985279513</v>
@@ -8835,7 +8835,7 @@
         <v>3</v>
       </c>
       <c r="M158">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="N158">
         <v>1.046608077533504</v>
@@ -8885,7 +8885,7 @@
         <v>4</v>
       </c>
       <c r="M159">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="N159">
         <v>-0.04238633276435765</v>
@@ -8935,7 +8935,7 @@
         <v>5</v>
       </c>
       <c r="M160">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="N160">
         <v>-1.153904848852118</v>
@@ -8985,7 +8985,7 @@
         <v>5</v>
       </c>
       <c r="M161">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="N161">
         <v>-0.6525445255282016</v>
@@ -9185,7 +9185,7 @@
         <v>5</v>
       </c>
       <c r="M165">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="N165">
         <v>-1.757518204989799</v>
@@ -9235,7 +9235,7 @@
         <v>4</v>
       </c>
       <c r="M166">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="N166">
         <v>0.7049558865422446</v>
@@ -9285,7 +9285,7 @@
         <v>5</v>
       </c>
       <c r="M167">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="N167">
         <v>-0.8773260658399902</v>
@@ -9335,7 +9335,7 @@
         <v>2</v>
       </c>
       <c r="M168">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="N168">
         <v>3.044527383230702</v>
@@ -9435,7 +9435,7 @@
         <v>4</v>
       </c>
       <c r="M170">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="N170">
         <v>-0.8318012892608124</v>

</xml_diff>